<commit_message>
Increased the effciency of lecture comparions so that it doesn't take 10 seconeds to calculate the schedule. Also fixed minor issue with test data
</commit_message>
<xml_diff>
--- a/SCE_ProgramsCourses (copy).xlsx
+++ b/SCE_ProgramsCourses (copy).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B104AECE-E94B-4C6C-96D0-F30F7E06A3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC72B3C-B7BD-4FA9-BE56-0B034A9C5D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="10140" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="3270" windowWidth="21600" windowHeight="10140" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Core Courses (PCOM)" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Program Specific Courses" sheetId="3" r:id="rId3"/>
     <sheet name="Classrooms" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
   <si>
     <t>Color Code</t>
   </si>
@@ -860,13 +860,31 @@
     <t>11-537</t>
   </si>
   <si>
-    <t>11-323 Computer Lab</t>
-  </si>
-  <si>
-    <t>11-324 Computer Lab</t>
-  </si>
-  <si>
-    <t>11-325 Computer Lab</t>
+    <t>11-538</t>
+  </si>
+  <si>
+    <t>11-539</t>
+  </si>
+  <si>
+    <t>11-5310</t>
+  </si>
+  <si>
+    <t>11-323C Computer Lab</t>
+  </si>
+  <si>
+    <t>11-324C Computer Lab</t>
+  </si>
+  <si>
+    <t>11-325C Computer Lab</t>
+  </si>
+  <si>
+    <t>11-625C Computer Lab</t>
+  </si>
+  <si>
+    <t>11-5312</t>
+  </si>
+  <si>
+    <t>11-329C Computer Lab</t>
   </si>
 </sst>
 </file>
@@ -1883,28 +1901,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1928,29 +1949,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2946,11 +2964,11 @@
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="140" t="s">
@@ -2960,11 +2978,11 @@
       <c r="C3" s="140"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="166" t="s">
+      <c r="A4" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="166"/>
-      <c r="C4" s="166"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="145"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
@@ -2975,48 +2993,48 @@
       </c>
       <c r="B6" s="142"/>
       <c r="C6" s="142"/>
-      <c r="D6" s="151" t="s">
+      <c r="D6" s="146" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="46"/>
-      <c r="F6" s="162" t="s">
+      <c r="F6" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="162"/>
-      <c r="H6" s="162"/>
-      <c r="I6" s="160" t="s">
+      <c r="G6" s="147"/>
+      <c r="H6" s="147"/>
+      <c r="I6" s="148" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="47"/>
-      <c r="K6" s="162" t="s">
+      <c r="K6" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="162"/>
-      <c r="M6" s="162"/>
-      <c r="N6" s="160" t="s">
+      <c r="L6" s="147"/>
+      <c r="M6" s="147"/>
+      <c r="N6" s="148" t="s">
         <v>5</v>
       </c>
       <c r="O6" s="48"/>
-      <c r="P6" s="162" t="s">
+      <c r="P6" s="147" t="s">
         <v>74</v>
       </c>
-      <c r="Q6" s="162"/>
-      <c r="R6" s="162"/>
-      <c r="S6" s="160" t="s">
+      <c r="Q6" s="147"/>
+      <c r="R6" s="147"/>
+      <c r="S6" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="161" t="s">
+      <c r="T6" s="149" t="s">
         <v>75</v>
       </c>
-      <c r="V6" s="162" t="s">
+      <c r="V6" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="162"/>
-      <c r="X6" s="162"/>
-      <c r="Y6" s="163" t="s">
+      <c r="W6" s="147"/>
+      <c r="X6" s="147"/>
+      <c r="Y6" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="164" t="s">
+      <c r="Z6" s="151" t="s">
         <v>75</v>
       </c>
       <c r="AB6" s="142" t="s">
@@ -3024,7 +3042,7 @@
       </c>
       <c r="AC6" s="142"/>
       <c r="AD6" s="142"/>
-      <c r="AE6" s="151" t="s">
+      <c r="AE6" s="146" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3032,79 +3050,79 @@
       <c r="A7" s="142"/>
       <c r="B7" s="142"/>
       <c r="C7" s="142"/>
-      <c r="D7" s="151"/>
+      <c r="D7" s="146"/>
       <c r="E7" s="46"/>
-      <c r="F7" s="162"/>
-      <c r="G7" s="162"/>
-      <c r="H7" s="162"/>
-      <c r="I7" s="160"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="148"/>
       <c r="J7" s="47"/>
-      <c r="K7" s="162"/>
-      <c r="L7" s="162"/>
-      <c r="M7" s="162"/>
-      <c r="N7" s="160"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="147"/>
+      <c r="M7" s="147"/>
+      <c r="N7" s="148"/>
       <c r="O7" s="48"/>
-      <c r="P7" s="162"/>
-      <c r="Q7" s="162"/>
-      <c r="R7" s="162"/>
-      <c r="S7" s="160"/>
-      <c r="T7" s="161"/>
-      <c r="V7" s="162"/>
-      <c r="W7" s="162"/>
-      <c r="X7" s="162"/>
-      <c r="Y7" s="163"/>
-      <c r="Z7" s="164"/>
+      <c r="P7" s="147"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="147"/>
+      <c r="S7" s="148"/>
+      <c r="T7" s="149"/>
+      <c r="V7" s="147"/>
+      <c r="W7" s="147"/>
+      <c r="X7" s="147"/>
+      <c r="Y7" s="150"/>
+      <c r="Z7" s="151"/>
       <c r="AB7" s="142"/>
       <c r="AC7" s="142"/>
       <c r="AD7" s="142"/>
-      <c r="AE7" s="151"/>
+      <c r="AE7" s="146"/>
     </row>
     <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="142"/>
       <c r="B8" s="142"/>
       <c r="C8" s="142"/>
-      <c r="D8" s="151"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="46"/>
-      <c r="F8" s="162"/>
-      <c r="G8" s="162"/>
-      <c r="H8" s="162"/>
-      <c r="I8" s="160"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="148"/>
       <c r="J8" s="47"/>
-      <c r="K8" s="162"/>
-      <c r="L8" s="162"/>
-      <c r="M8" s="162"/>
-      <c r="N8" s="160"/>
+      <c r="K8" s="147"/>
+      <c r="L8" s="147"/>
+      <c r="M8" s="147"/>
+      <c r="N8" s="148"/>
       <c r="O8" s="48"/>
-      <c r="P8" s="162"/>
-      <c r="Q8" s="162"/>
-      <c r="R8" s="162"/>
-      <c r="S8" s="160"/>
-      <c r="T8" s="161"/>
-      <c r="V8" s="162"/>
-      <c r="W8" s="162"/>
-      <c r="X8" s="162"/>
-      <c r="Y8" s="163"/>
-      <c r="Z8" s="164"/>
+      <c r="P8" s="147"/>
+      <c r="Q8" s="147"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="148"/>
+      <c r="T8" s="149"/>
+      <c r="V8" s="147"/>
+      <c r="W8" s="147"/>
+      <c r="X8" s="147"/>
+      <c r="Y8" s="150"/>
+      <c r="Z8" s="151"/>
       <c r="AB8" s="142"/>
       <c r="AC8" s="142"/>
       <c r="AD8" s="142"/>
-      <c r="AE8" s="151"/>
+      <c r="AE8" s="146"/>
     </row>
     <row r="9" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="146" t="s">
+      <c r="A9" s="152" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="153" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="153" t="s">
+      <c r="C9" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="154">
+      <c r="D9" s="155">
         <v>21</v>
       </c>
       <c r="E9" s="50"/>
-      <c r="F9" s="155" t="s">
+      <c r="F9" s="156" t="s">
         <v>78</v>
       </c>
       <c r="G9" s="51" t="s">
@@ -3130,7 +3148,7 @@
         <v>21</v>
       </c>
       <c r="O9" s="55"/>
-      <c r="P9" s="156" t="s">
+      <c r="P9" s="157" t="s">
         <v>78</v>
       </c>
       <c r="Q9" s="51" t="s">
@@ -3166,12 +3184,12 @@
       </c>
     </row>
     <row r="10" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="146"/>
-      <c r="B10" s="152"/>
-      <c r="C10" s="153"/>
-      <c r="D10" s="154"/>
+      <c r="A10" s="152"/>
+      <c r="B10" s="153"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="155"/>
       <c r="E10" s="50"/>
-      <c r="F10" s="155"/>
+      <c r="F10" s="156"/>
       <c r="G10" s="7" t="s">
         <v>89</v>
       </c>
@@ -3193,7 +3211,7 @@
         <v>21</v>
       </c>
       <c r="O10" s="55"/>
-      <c r="P10" s="156"/>
+      <c r="P10" s="157"/>
       <c r="Q10" s="7" t="s">
         <v>93</v>
       </c>
@@ -3229,25 +3247,25 @@
       </c>
     </row>
     <row r="11" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="146"/>
-      <c r="B11" s="157" t="s">
+      <c r="A11" s="152"/>
+      <c r="B11" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="158" t="s">
+      <c r="C11" s="159" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="144">
+      <c r="D11" s="160">
         <v>14</v>
       </c>
       <c r="E11" s="73"/>
-      <c r="F11" s="155"/>
-      <c r="G11" s="159" t="s">
+      <c r="F11" s="156"/>
+      <c r="G11" s="161" t="s">
         <v>101</v>
       </c>
-      <c r="H11" s="158" t="s">
+      <c r="H11" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="144">
+      <c r="I11" s="160">
         <v>21</v>
       </c>
       <c r="J11" s="54"/>
@@ -3262,7 +3280,7 @@
         <v>15</v>
       </c>
       <c r="O11" s="55"/>
-      <c r="P11" s="156"/>
+      <c r="P11" s="157"/>
       <c r="Q11" s="7" t="s">
         <v>105</v>
       </c>
@@ -3300,15 +3318,15 @@
       </c>
     </row>
     <row r="12" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="146"/>
-      <c r="B12" s="157"/>
-      <c r="C12" s="158"/>
-      <c r="D12" s="144"/>
+      <c r="A12" s="152"/>
+      <c r="B12" s="158"/>
+      <c r="C12" s="159"/>
+      <c r="D12" s="160"/>
       <c r="E12" s="73"/>
-      <c r="F12" s="155"/>
-      <c r="G12" s="159"/>
-      <c r="H12" s="158"/>
-      <c r="I12" s="144"/>
+      <c r="F12" s="156"/>
+      <c r="G12" s="161"/>
+      <c r="H12" s="159"/>
+      <c r="I12" s="160"/>
       <c r="J12" s="54"/>
       <c r="K12" s="138"/>
       <c r="L12" s="7" t="s">
@@ -3321,7 +3339,7 @@
         <v>50</v>
       </c>
       <c r="O12" s="55"/>
-      <c r="P12" s="156"/>
+      <c r="P12" s="157"/>
       <c r="Q12" s="7" t="s">
         <v>114</v>
       </c>
@@ -3360,7 +3378,7 @@
       </c>
     </row>
     <row r="13" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="146"/>
+      <c r="A13" s="152"/>
       <c r="B13" s="72" t="s">
         <v>120</v>
       </c>
@@ -3371,7 +3389,7 @@
         <v>21</v>
       </c>
       <c r="E13" s="73"/>
-      <c r="F13" s="155"/>
+      <c r="F13" s="156"/>
       <c r="G13" s="7" t="s">
         <v>122</v>
       </c>
@@ -3392,7 +3410,7 @@
         <v>107</v>
       </c>
       <c r="O13" s="55"/>
-      <c r="P13" s="156"/>
+      <c r="P13" s="157"/>
       <c r="Q13" s="7" t="s">
         <v>125</v>
       </c>
@@ -3417,7 +3435,7 @@
       </c>
       <c r="Z13" s="82"/>
       <c r="AA13" s="83"/>
-      <c r="AB13" s="145" t="s">
+      <c r="AB13" s="162" t="s">
         <v>18</v>
       </c>
       <c r="AC13" s="51" t="s">
@@ -3431,7 +3449,7 @@
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="146"/>
+      <c r="A14" s="152"/>
       <c r="B14" s="55"/>
       <c r="C14" s="86" t="s">
         <v>131</v>
@@ -3441,7 +3459,7 @@
         <v>56</v>
       </c>
       <c r="E14" s="88"/>
-      <c r="F14" s="155"/>
+      <c r="F14" s="156"/>
       <c r="G14" s="89"/>
       <c r="H14" s="90" t="s">
         <v>132</v>
@@ -3464,7 +3482,7 @@
         <v>15</v>
       </c>
       <c r="O14" s="55"/>
-      <c r="P14" s="156"/>
+      <c r="P14" s="157"/>
       <c r="Q14" s="80"/>
       <c r="R14" s="76" t="s">
         <v>135</v>
@@ -3489,7 +3507,7 @@
       </c>
       <c r="Z14" s="96"/>
       <c r="AA14" s="59"/>
-      <c r="AB14" s="145"/>
+      <c r="AB14" s="162"/>
       <c r="AC14" s="51" t="s">
         <v>138</v>
       </c>
@@ -3501,7 +3519,7 @@
       </c>
     </row>
     <row r="15" spans="1:31" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="146" t="s">
+      <c r="A15" s="152" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="98" t="s">
@@ -3514,7 +3532,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="50"/>
-      <c r="F15" s="147" t="s">
+      <c r="F15" s="163" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -3565,7 +3583,7 @@
         <v>18</v>
       </c>
       <c r="Z15" s="100"/>
-      <c r="AB15" s="145"/>
+      <c r="AB15" s="162"/>
       <c r="AC15" s="51" t="s">
         <v>151</v>
       </c>
@@ -3577,7 +3595,7 @@
       </c>
     </row>
     <row r="16" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="146"/>
+      <c r="A16" s="152"/>
       <c r="B16" s="81" t="s">
         <v>153</v>
       </c>
@@ -3588,7 +3606,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="50"/>
-      <c r="F16" s="147"/>
+      <c r="F16" s="163"/>
       <c r="G16" s="7" t="s">
         <v>155</v>
       </c>
@@ -3638,7 +3656,7 @@
         <v>164</v>
       </c>
       <c r="AA16" s="59"/>
-      <c r="AB16" s="145"/>
+      <c r="AB16" s="162"/>
       <c r="AC16" s="76"/>
       <c r="AD16" s="77" t="s">
         <v>165</v>
@@ -3649,7 +3667,7 @@
       </c>
     </row>
     <row r="17" spans="1:31" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="146"/>
+      <c r="A17" s="152"/>
       <c r="B17" s="81" t="s">
         <v>166</v>
       </c>
@@ -3660,7 +3678,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="50"/>
-      <c r="F17" s="147"/>
+      <c r="F17" s="163"/>
       <c r="G17" s="16" t="s">
         <v>168</v>
       </c>
@@ -3709,7 +3727,7 @@
         <v>162</v>
       </c>
       <c r="AA17" s="59"/>
-      <c r="AB17" s="148" t="s">
+      <c r="AB17" s="164" t="s">
         <v>26</v>
       </c>
       <c r="AC17" s="51" t="s">
@@ -3723,7 +3741,7 @@
       </c>
     </row>
     <row r="18" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="146"/>
+      <c r="A18" s="152"/>
       <c r="B18" s="81" t="s">
         <v>178</v>
       </c>
@@ -3734,7 +3752,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="50"/>
-      <c r="F18" s="147"/>
+      <c r="F18" s="163"/>
       <c r="G18" s="89"/>
       <c r="H18" s="90" t="s">
         <v>180</v>
@@ -3744,7 +3762,7 @@
         <v>70</v>
       </c>
       <c r="J18" s="54"/>
-      <c r="K18" s="149" t="s">
+      <c r="K18" s="165" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="92" t="s">
@@ -3782,7 +3800,7 @@
       </c>
       <c r="Z18" s="108"/>
       <c r="AA18" s="109"/>
-      <c r="AB18" s="148"/>
+      <c r="AB18" s="164"/>
       <c r="AC18" s="51" t="s">
         <v>187</v>
       </c>
@@ -3794,7 +3812,7 @@
       </c>
     </row>
     <row r="19" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="146"/>
+      <c r="A19" s="152"/>
       <c r="B19" s="55"/>
       <c r="C19" s="86" t="s">
         <v>189</v>
@@ -3817,7 +3835,7 @@
         <v>14</v>
       </c>
       <c r="J19" s="54"/>
-      <c r="K19" s="149"/>
+      <c r="K19" s="165"/>
       <c r="L19" s="7" t="s">
         <v>192</v>
       </c>
@@ -3856,7 +3874,7 @@
       </c>
       <c r="Z19" s="96"/>
       <c r="AA19" s="59"/>
-      <c r="AB19" s="148"/>
+      <c r="AB19" s="164"/>
       <c r="AC19" s="76"/>
       <c r="AD19" s="77" t="s">
         <v>199</v>
@@ -3867,7 +3885,7 @@
       </c>
     </row>
     <row r="20" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="150" t="s">
+      <c r="A20" s="166" t="s">
         <v>200</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3891,7 +3909,7 @@
         <v>39</v>
       </c>
       <c r="J20" s="54"/>
-      <c r="K20" s="149"/>
+      <c r="K20" s="165"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76" t="s">
         <v>205</v>
@@ -3926,7 +3944,7 @@
       <c r="AA20" s="59"/>
     </row>
     <row r="21" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
+      <c r="A21" s="166"/>
       <c r="B21" s="8" t="s">
         <v>209</v>
       </c>
@@ -3979,7 +3997,7 @@
       <c r="AB21" s="115"/>
     </row>
     <row r="22" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
+      <c r="A22" s="166"/>
       <c r="B22" s="80"/>
       <c r="C22" s="76" t="s">
         <v>217</v>
@@ -4229,21 +4247,19 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="F6:H8"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="K6:M8"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="P6:R8"/>
-    <mergeCell ref="S6:S8"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="V6:X8"/>
-    <mergeCell ref="Y6:Y8"/>
-    <mergeCell ref="Z6:Z8"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="AB13:AB16"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="V14:V18"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="P15:P20"/>
+    <mergeCell ref="AB17:AB19"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="V19:V22"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="P21:P22"/>
     <mergeCell ref="AB6:AD8"/>
     <mergeCell ref="AE6:AE8"/>
     <mergeCell ref="A9:A14"/>
@@ -4260,19 +4276,21 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="AB13:AB16"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="V14:V18"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="P15:P20"/>
-    <mergeCell ref="AB17:AB19"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="V19:V22"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="S6:S8"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="V6:X8"/>
+    <mergeCell ref="Y6:Y8"/>
+    <mergeCell ref="Z6:Z8"/>
+    <mergeCell ref="F6:H8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="K6:M8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="P6:R8"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C8"/>
+    <mergeCell ref="D6:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4281,10 +4299,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ11"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4320,7 +4338,7 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B4">
         <v>36</v>
@@ -4336,7 +4354,7 @@
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B6">
         <v>30</v>
@@ -4352,7 +4370,7 @@
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B8">
         <v>24</v>
@@ -4368,15 +4386,51 @@
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B10">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
+      <c r="A11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Revert "Updated warnings for having too many students and not selecting a semester"
</commit_message>
<xml_diff>
--- a/SCE_ProgramsCourses (copy).xlsx
+++ b/SCE_ProgramsCourses (copy).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\2023-01_Team6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC72B3C-B7BD-4FA9-BE56-0B034A9C5D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBC2D38-02B5-45D1-A17E-958487C3A544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="3270" windowWidth="21600" windowHeight="10140" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Core Courses (PCOM)" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="255">
   <si>
     <t>Color Code</t>
   </si>
@@ -866,25 +866,82 @@
     <t>11-539</t>
   </si>
   <si>
-    <t>11-5310</t>
-  </si>
-  <si>
-    <t>11-323C Computer Lab</t>
-  </si>
-  <si>
-    <t>11-324C Computer Lab</t>
-  </si>
-  <si>
-    <t>11-325C Computer Lab</t>
-  </si>
-  <si>
-    <t>11-625C Computer Lab</t>
-  </si>
-  <si>
-    <t>11-5312</t>
-  </si>
-  <si>
-    <t>11-329C Computer Lab</t>
+    <t>11-540</t>
+  </si>
+  <si>
+    <t>11-541</t>
+  </si>
+  <si>
+    <t>11-542</t>
+  </si>
+  <si>
+    <t>11-543</t>
+  </si>
+  <si>
+    <t>11-544</t>
+  </si>
+  <si>
+    <t>11-545</t>
+  </si>
+  <si>
+    <t>11-546</t>
+  </si>
+  <si>
+    <t>11-547</t>
+  </si>
+  <si>
+    <t>11-548</t>
+  </si>
+  <si>
+    <t>11-549</t>
+  </si>
+  <si>
+    <t>11-550</t>
+  </si>
+  <si>
+    <t>11-551</t>
+  </si>
+  <si>
+    <t>11-552</t>
+  </si>
+  <si>
+    <t>11-553</t>
+  </si>
+  <si>
+    <t>11-554</t>
+  </si>
+  <si>
+    <t>11-555</t>
+  </si>
+  <si>
+    <t>11-556</t>
+  </si>
+  <si>
+    <t>11-557</t>
+  </si>
+  <si>
+    <t>11-558</t>
+  </si>
+  <si>
+    <t>11-559</t>
+  </si>
+  <si>
+    <t>11-560</t>
+  </si>
+  <si>
+    <t>11-561 Lab</t>
+  </si>
+  <si>
+    <t>11-562 Lab</t>
+  </si>
+  <si>
+    <t>11-563 Lab</t>
+  </si>
+  <si>
+    <t>11-564 Lab</t>
+  </si>
+  <si>
+    <t>11-565 Lab</t>
   </si>
 </sst>
 </file>
@@ -897,7 +954,7 @@
     <numFmt numFmtId="166" formatCode="\$#,##0.00_);[Red]&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="167" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -997,6 +1054,12 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1486,11 +1549,53 @@
   </cellStyleXfs>
   <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1879,48 +1984,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2368,211 +2431,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="140"/>
-      <c r="C3" s="140"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="141" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="141"/>
-      <c r="C4" s="141"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="16"/>
     </row>
     <row r="6" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="142" t="s">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="142"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="1" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="137" t="s">
+      <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="20">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="137"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="23">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="137"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="23">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="137"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="23">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="137"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="23">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="137"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="28">
         <f>SUM(D7:D11)</f>
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="137" t="s">
+      <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="20">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="137"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="32">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="137"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="23">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="137"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="35">
         <f>SUM(D13:D15)</f>
         <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="138" t="s">
+      <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="37">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="138"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="23">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="138"/>
-      <c r="B19" s="24" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="23">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="138"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="27" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="42">
         <f>SUM(D17:D19)</f>
         <v>82</v>
       </c>
@@ -2609,295 +2672,295 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="140"/>
-      <c r="C3" s="140"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="141" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="141"/>
-      <c r="C4" s="141"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="16"/>
     </row>
     <row r="6" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="142" t="s">
+      <c r="A6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="142"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="1" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="137" t="s">
+      <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="20">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="137"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="23">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="137"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="23">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="137"/>
-      <c r="B10" s="29" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="23">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="137"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="23">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="137"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="23">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="137"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="28">
         <f>SUM(D7:D12)</f>
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143" t="s">
+      <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="143"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="23">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="23">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="23">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="143"/>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="143"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="23">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="143"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="13" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="28">
         <f>SUM(D14:D19)</f>
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="143" t="s">
+      <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="37">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
-      <c r="B22" s="34" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="50">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="143"/>
-      <c r="B23" s="34" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="50">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="143"/>
-      <c r="B24" s="34" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="50">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="143"/>
-      <c r="B25" s="34" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="23">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="143"/>
-      <c r="B26" s="37" t="s">
+      <c r="A26" s="8"/>
+      <c r="B26" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="39">
+      <c r="D26" s="53">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="143"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="41" t="s">
+      <c r="A27" s="8"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="56">
         <f>SUM(D21:D26)</f>
         <v>76</v>
       </c>
@@ -2927,186 +2990,186 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="43" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="43" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" style="43" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="43" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="43" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="43" customWidth="1"/>
-    <col min="8" max="8" width="38.42578125" style="43" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="43" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="43" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="43" customWidth="1"/>
-    <col min="13" max="13" width="39.42578125" style="43" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="43" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" style="43" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="43" customWidth="1"/>
-    <col min="18" max="18" width="43" style="43" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="43" customWidth="1"/>
-    <col min="20" max="20" width="58.42578125" style="43" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="43" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" style="43" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" style="43" customWidth="1"/>
-    <col min="24" max="24" width="26.5703125" style="43" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" style="43" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" style="43" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" style="43" customWidth="1"/>
-    <col min="28" max="28" width="7.5703125" style="43" customWidth="1"/>
-    <col min="29" max="29" width="8.85546875" style="43" customWidth="1"/>
-    <col min="30" max="30" width="39.85546875" style="43" customWidth="1"/>
-    <col min="31" max="31" width="13.5703125" style="43" customWidth="1"/>
-    <col min="32" max="1024" width="9.42578125" style="43"/>
+    <col min="1" max="1" width="7.5703125" style="57" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="57" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" style="57" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="57" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="57" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="57" customWidth="1"/>
+    <col min="8" max="8" width="38.42578125" style="57" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="57" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="57" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="57" customWidth="1"/>
+    <col min="13" max="13" width="39.42578125" style="57" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="57" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" style="57" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="57" customWidth="1"/>
+    <col min="18" max="18" width="43" style="57" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="57" customWidth="1"/>
+    <col min="20" max="20" width="58.42578125" style="57" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="57" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" style="57" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" style="57" customWidth="1"/>
+    <col min="24" max="24" width="26.5703125" style="57" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="57" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" style="57" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="57" customWidth="1"/>
+    <col min="28" max="28" width="7.5703125" style="57" customWidth="1"/>
+    <col min="29" max="29" width="8.85546875" style="57" customWidth="1"/>
+    <col min="30" max="30" width="39.85546875" style="57" customWidth="1"/>
+    <col min="31" max="31" width="13.5703125" style="57" customWidth="1"/>
+    <col min="32" max="1024" width="9.42578125" style="57"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="144"/>
-      <c r="C2" s="144"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="140"/>
-      <c r="C3" s="140"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="145" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="145"/>
-      <c r="C4" s="145"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="59"/>
     </row>
     <row r="6" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="142" t="s">
+      <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="142"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="146" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="147" t="s">
+      <c r="E6" s="60"/>
+      <c r="F6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="147"/>
-      <c r="H6" s="147"/>
-      <c r="I6" s="148" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="47"/>
-      <c r="K6" s="147" t="s">
+      <c r="J6" s="61"/>
+      <c r="K6" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="147"/>
-      <c r="M6" s="147"/>
-      <c r="N6" s="148" t="s">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="48"/>
-      <c r="P6" s="147" t="s">
+      <c r="O6" s="62"/>
+      <c r="P6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q6" s="147"/>
-      <c r="R6" s="147"/>
-      <c r="S6" s="148" t="s">
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="149" t="s">
+      <c r="T6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="V6" s="147" t="s">
+      <c r="V6" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="147"/>
-      <c r="X6" s="147"/>
-      <c r="Y6" s="150" t="s">
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Z6" s="151" t="s">
         <v>75</v>
       </c>
-      <c r="AB6" s="142" t="s">
+      <c r="AB6" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="AC6" s="142"/>
-      <c r="AD6" s="142"/>
-      <c r="AE6" s="146" t="s">
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="142"/>
-      <c r="B7" s="142"/>
-      <c r="C7" s="142"/>
-      <c r="D7" s="146"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="147"/>
-      <c r="H7" s="147"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="147"/>
-      <c r="L7" s="147"/>
-      <c r="M7" s="147"/>
-      <c r="N7" s="148"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="147"/>
-      <c r="R7" s="147"/>
-      <c r="S7" s="148"/>
-      <c r="T7" s="149"/>
-      <c r="V7" s="147"/>
-      <c r="W7" s="147"/>
-      <c r="X7" s="147"/>
-      <c r="Y7" s="150"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="2"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="1"/>
       <c r="Z7" s="151"/>
-      <c r="AB7" s="142"/>
-      <c r="AC7" s="142"/>
-      <c r="AD7" s="142"/>
-      <c r="AE7" s="146"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="5"/>
     </row>
     <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="142"/>
-      <c r="B8" s="142"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="146"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="147"/>
-      <c r="H8" s="147"/>
-      <c r="I8" s="148"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="147"/>
-      <c r="L8" s="147"/>
-      <c r="M8" s="147"/>
-      <c r="N8" s="148"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="147"/>
-      <c r="Q8" s="147"/>
-      <c r="R8" s="147"/>
-      <c r="S8" s="148"/>
-      <c r="T8" s="149"/>
-      <c r="V8" s="147"/>
-      <c r="W8" s="147"/>
-      <c r="X8" s="147"/>
-      <c r="Y8" s="150"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="62"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="2"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="1"/>
       <c r="Z8" s="151"/>
-      <c r="AB8" s="142"/>
-      <c r="AC8" s="142"/>
-      <c r="AD8" s="142"/>
-      <c r="AE8" s="146"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="5"/>
     </row>
     <row r="9" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="152" t="s">
@@ -3121,65 +3184,65 @@
       <c r="D9" s="155">
         <v>21</v>
       </c>
-      <c r="E9" s="50"/>
+      <c r="E9" s="64"/>
       <c r="F9" s="156" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G9" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="52" t="s">
+      <c r="H9" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="53">
+      <c r="I9" s="67">
         <v>21</v>
       </c>
-      <c r="J9" s="54"/>
-      <c r="K9" s="138" t="s">
+      <c r="J9" s="68"/>
+      <c r="K9" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="20">
         <v>21</v>
       </c>
-      <c r="O9" s="55"/>
+      <c r="O9" s="69"/>
       <c r="P9" s="157" t="s">
         <v>78</v>
       </c>
-      <c r="Q9" s="51" t="s">
+      <c r="Q9" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="R9" s="56" t="s">
+      <c r="R9" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="S9" s="57">
+      <c r="S9" s="71">
         <v>16</v>
       </c>
-      <c r="T9" s="58"/>
-      <c r="U9" s="59"/>
-      <c r="V9" s="138" t="s">
+      <c r="T9" s="72"/>
+      <c r="U9" s="73"/>
+      <c r="V9" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="W9" s="60"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="62"/>
-      <c r="AB9" s="138" t="s">
+      <c r="W9" s="74"/>
+      <c r="X9" s="74"/>
+      <c r="Y9" s="74"/>
+      <c r="Z9" s="75"/>
+      <c r="AA9" s="76"/>
+      <c r="AB9" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="4" t="s">
+      <c r="AC9" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="AD9" s="63" t="s">
+      <c r="AD9" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="AE9" s="64">
+      <c r="AE9" s="78">
         <v>18</v>
       </c>
     </row>
@@ -3188,61 +3251,61 @@
       <c r="B10" s="153"/>
       <c r="C10" s="154"/>
       <c r="D10" s="155"/>
-      <c r="E10" s="50"/>
+      <c r="E10" s="64"/>
       <c r="F10" s="156"/>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="I10" s="65">
+      <c r="I10" s="79">
         <v>14</v>
       </c>
-      <c r="J10" s="54"/>
-      <c r="K10" s="138"/>
-      <c r="L10" s="7" t="s">
+      <c r="J10" s="68"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="M10" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="23">
         <v>21</v>
       </c>
-      <c r="O10" s="55"/>
+      <c r="O10" s="69"/>
       <c r="P10" s="157"/>
-      <c r="Q10" s="7" t="s">
+      <c r="Q10" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="R10" s="66" t="s">
+      <c r="R10" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="S10" s="67">
+      <c r="S10" s="81">
         <v>16</v>
       </c>
-      <c r="T10" s="58"/>
-      <c r="U10" s="59"/>
-      <c r="V10" s="138"/>
-      <c r="W10" s="7" t="s">
+      <c r="T10" s="72"/>
+      <c r="U10" s="73"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="X10" s="66" t="s">
+      <c r="X10" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="Y10" s="68">
+      <c r="Y10" s="82">
         <v>18</v>
       </c>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="62"/>
-      <c r="AB10" s="138"/>
-      <c r="AC10" s="7" t="s">
+      <c r="Z10" s="83"/>
+      <c r="AA10" s="76"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="AD10" s="70" t="s">
+      <c r="AD10" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="AE10" s="71">
+      <c r="AE10" s="85">
         <v>12</v>
       </c>
     </row>
@@ -3257,7 +3320,7 @@
       <c r="D11" s="160">
         <v>14</v>
       </c>
-      <c r="E11" s="73"/>
+      <c r="E11" s="87"/>
       <c r="F11" s="156"/>
       <c r="G11" s="161" t="s">
         <v>101</v>
@@ -3268,52 +3331,52 @@
       <c r="I11" s="160">
         <v>21</v>
       </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="138"/>
-      <c r="L11" s="7" t="s">
+      <c r="J11" s="68"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="23">
         <v>15</v>
       </c>
-      <c r="O11" s="55"/>
+      <c r="O11" s="69"/>
       <c r="P11" s="157"/>
-      <c r="Q11" s="7" t="s">
+      <c r="Q11" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="R11" s="66" t="s">
+      <c r="R11" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="S11" s="67">
+      <c r="S11" s="81">
         <v>16</v>
       </c>
-      <c r="T11" s="74" t="s">
+      <c r="T11" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="U11" s="59"/>
-      <c r="V11" s="138"/>
-      <c r="W11" s="7" t="s">
+      <c r="U11" s="73"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="X11" s="66" t="s">
+      <c r="X11" s="80" t="s">
         <v>109</v>
       </c>
-      <c r="Y11" s="68">
+      <c r="Y11" s="82">
         <v>24</v>
       </c>
-      <c r="Z11" s="69"/>
-      <c r="AA11" s="62"/>
-      <c r="AB11" s="138"/>
-      <c r="AC11" s="7" t="s">
+      <c r="Z11" s="83"/>
+      <c r="AA11" s="76"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="AD11" s="70" t="s">
+      <c r="AD11" s="84" t="s">
         <v>111</v>
       </c>
-      <c r="AE11" s="71">
+      <c r="AE11" s="85">
         <v>12</v>
       </c>
     </row>
@@ -3322,199 +3385,199 @@
       <c r="B12" s="158"/>
       <c r="C12" s="159"/>
       <c r="D12" s="160"/>
-      <c r="E12" s="73"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="156"/>
       <c r="G12" s="161"/>
       <c r="H12" s="159"/>
       <c r="I12" s="160"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="138"/>
-      <c r="L12" s="7" t="s">
+      <c r="J12" s="68"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="M12" s="75" t="s">
+      <c r="M12" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="23">
         <v>50</v>
       </c>
-      <c r="O12" s="55"/>
+      <c r="O12" s="69"/>
       <c r="P12" s="157"/>
-      <c r="Q12" s="7" t="s">
+      <c r="Q12" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="R12" s="66" t="s">
+      <c r="R12" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="S12" s="67">
+      <c r="S12" s="81">
         <v>16</v>
       </c>
-      <c r="T12" s="58" t="s">
+      <c r="T12" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="U12" s="59"/>
-      <c r="V12" s="138"/>
-      <c r="W12" s="7" t="s">
+      <c r="U12" s="73"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="X12" s="66" t="s">
+      <c r="X12" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="Y12" s="68">
+      <c r="Y12" s="82">
         <v>24</v>
       </c>
-      <c r="Z12" s="69" t="s">
+      <c r="Z12" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="AA12" s="62"/>
-      <c r="AB12" s="138"/>
-      <c r="AC12" s="76"/>
-      <c r="AD12" s="77" t="s">
+      <c r="AA12" s="76"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="90"/>
+      <c r="AD12" s="91" t="s">
         <v>119</v>
       </c>
-      <c r="AE12" s="78">
+      <c r="AE12" s="92">
         <f>SUM(AE9:AE11)</f>
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="152"/>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="65">
+      <c r="D13" s="79">
         <v>21</v>
       </c>
-      <c r="E13" s="73"/>
+      <c r="E13" s="87"/>
       <c r="F13" s="156"/>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="I13" s="65">
+      <c r="I13" s="79">
         <v>14</v>
       </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="138"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="76" t="s">
+      <c r="J13" s="68"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="90" t="s">
         <v>124</v>
       </c>
-      <c r="N13" s="77">
+      <c r="N13" s="91">
         <f>SUM(N9:N12)</f>
         <v>107</v>
       </c>
-      <c r="O13" s="55"/>
+      <c r="O13" s="69"/>
       <c r="P13" s="157"/>
-      <c r="Q13" s="7" t="s">
+      <c r="Q13" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="R13" s="66" t="s">
+      <c r="R13" s="80" t="s">
         <v>126</v>
       </c>
-      <c r="S13" s="67">
+      <c r="S13" s="81">
         <v>16</v>
       </c>
-      <c r="T13" s="81" t="s">
+      <c r="T13" s="95" t="s">
         <v>127</v>
       </c>
-      <c r="U13" s="59"/>
-      <c r="V13" s="138"/>
-      <c r="W13" s="80"/>
-      <c r="X13" s="76" t="s">
+      <c r="U13" s="73"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="94"/>
+      <c r="X13" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="Y13" s="77">
+      <c r="Y13" s="91">
         <f>SUM(Y9:Y12)</f>
         <v>66</v>
       </c>
-      <c r="Z13" s="82"/>
-      <c r="AA13" s="83"/>
+      <c r="Z13" s="96"/>
+      <c r="AA13" s="97"/>
       <c r="AB13" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="AC13" s="51" t="s">
+      <c r="AC13" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="AD13" s="84" t="s">
+      <c r="AD13" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="AE13" s="85">
+      <c r="AE13" s="99">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="152"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="86" t="s">
+      <c r="B14" s="69"/>
+      <c r="C14" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="87">
+      <c r="D14" s="101">
         <f>SUM(D9:D13)</f>
         <v>56</v>
       </c>
-      <c r="E14" s="88"/>
+      <c r="E14" s="102"/>
       <c r="F14" s="156"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="90" t="s">
+      <c r="G14" s="103"/>
+      <c r="H14" s="104" t="s">
         <v>132</v>
       </c>
-      <c r="I14" s="91">
+      <c r="I14" s="105">
         <f>SUM(I9:I13)</f>
         <v>70</v>
       </c>
-      <c r="J14" s="54"/>
-      <c r="K14" s="138" t="s">
+      <c r="J14" s="68"/>
+      <c r="K14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="M14" s="92" t="s">
+      <c r="M14" s="106" t="s">
         <v>134</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="20">
         <v>15</v>
       </c>
-      <c r="O14" s="55"/>
+      <c r="O14" s="69"/>
       <c r="P14" s="157"/>
-      <c r="Q14" s="80"/>
-      <c r="R14" s="76" t="s">
+      <c r="Q14" s="94"/>
+      <c r="R14" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="S14" s="77">
+      <c r="S14" s="91">
         <f>SUM(S9:S13)</f>
         <v>80</v>
       </c>
-      <c r="T14" s="93"/>
-      <c r="U14" s="83"/>
-      <c r="V14" s="137" t="s">
+      <c r="T14" s="107"/>
+      <c r="U14" s="97"/>
+      <c r="V14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="W14" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="X14" s="94" t="s">
+      <c r="X14" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="Y14" s="95">
+      <c r="Y14" s="109">
         <v>18</v>
       </c>
-      <c r="Z14" s="96"/>
-      <c r="AA14" s="59"/>
+      <c r="Z14" s="110"/>
+      <c r="AA14" s="73"/>
       <c r="AB14" s="162"/>
-      <c r="AC14" s="51" t="s">
+      <c r="AC14" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="AD14" s="66" t="s">
+      <c r="AD14" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="AE14" s="97">
+      <c r="AE14" s="111">
         <v>28</v>
       </c>
     </row>
@@ -3522,364 +3585,364 @@
       <c r="A15" s="152" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D15" s="63">
         <v>14</v>
       </c>
-      <c r="E15" s="50"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="I15" s="49">
+      <c r="I15" s="63">
         <v>21</v>
       </c>
-      <c r="J15" s="54"/>
-      <c r="K15" s="138"/>
-      <c r="L15" s="7" t="s">
+      <c r="J15" s="68"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="M15" s="8" t="s">
+      <c r="M15" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="23">
         <v>21</v>
       </c>
-      <c r="O15" s="55"/>
-      <c r="P15" s="138" t="s">
+      <c r="O15" s="69"/>
+      <c r="P15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Q15" s="4" t="s">
+      <c r="Q15" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="R15" s="94" t="s">
+      <c r="R15" s="108" t="s">
         <v>147</v>
       </c>
-      <c r="S15" s="99">
+      <c r="S15" s="113">
         <v>18</v>
       </c>
-      <c r="T15" s="58" t="s">
+      <c r="T15" s="72" t="s">
         <v>148</v>
       </c>
-      <c r="U15" s="59"/>
-      <c r="V15" s="137"/>
-      <c r="W15" s="7" t="s">
+      <c r="U15" s="73"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="X15" s="66" t="s">
+      <c r="X15" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="Y15" s="68">
+      <c r="Y15" s="82">
         <v>18</v>
       </c>
-      <c r="Z15" s="100"/>
+      <c r="Z15" s="114"/>
       <c r="AB15" s="162"/>
-      <c r="AC15" s="51" t="s">
+      <c r="AC15" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="AD15" s="66" t="s">
+      <c r="AD15" s="80" t="s">
         <v>152</v>
       </c>
-      <c r="AE15" s="67">
+      <c r="AE15" s="81">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="152"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="95" t="s">
         <v>153</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="D16" s="101">
+      <c r="D16" s="115">
         <v>21</v>
       </c>
-      <c r="E16" s="50"/>
+      <c r="E16" s="64"/>
       <c r="F16" s="163"/>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="I16" s="65">
+      <c r="I16" s="79">
         <v>14</v>
       </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="138"/>
-      <c r="L16" s="7" t="s">
+      <c r="J16" s="68"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="M16" s="75" t="s">
+      <c r="M16" s="89" t="s">
         <v>158</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="23">
         <v>50</v>
       </c>
-      <c r="O16" s="55"/>
-      <c r="P16" s="138"/>
-      <c r="Q16" s="7" t="s">
+      <c r="O16" s="69"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="R16" s="66" t="s">
+      <c r="R16" s="80" t="s">
         <v>160</v>
       </c>
-      <c r="S16" s="67">
+      <c r="S16" s="81">
         <v>16</v>
       </c>
-      <c r="T16" s="74" t="s">
+      <c r="T16" s="88" t="s">
         <v>161</v>
       </c>
-      <c r="U16" s="59"/>
-      <c r="V16" s="137"/>
-      <c r="W16" s="7" t="s">
+      <c r="U16" s="73"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="X16" s="66" t="s">
+      <c r="X16" s="80" t="s">
         <v>163</v>
       </c>
-      <c r="Y16" s="68">
+      <c r="Y16" s="82">
         <v>24</v>
       </c>
-      <c r="Z16" s="102" t="s">
+      <c r="Z16" s="116" t="s">
         <v>164</v>
       </c>
-      <c r="AA16" s="59"/>
+      <c r="AA16" s="73"/>
       <c r="AB16" s="162"/>
-      <c r="AC16" s="76"/>
-      <c r="AD16" s="77" t="s">
+      <c r="AC16" s="90"/>
+      <c r="AD16" s="91" t="s">
         <v>165</v>
       </c>
-      <c r="AE16" s="78">
+      <c r="AE16" s="92">
         <f>SUM(AE13:AE15)</f>
         <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="152"/>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="95" t="s">
         <v>166</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="89" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="79">
         <v>21</v>
       </c>
-      <c r="E17" s="50"/>
+      <c r="E17" s="64"/>
       <c r="F17" s="163"/>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="H17" s="103" t="s">
+      <c r="H17" s="117" t="s">
         <v>169</v>
       </c>
-      <c r="I17" s="104">
+      <c r="I17" s="118">
         <v>35</v>
       </c>
-      <c r="J17" s="54"/>
-      <c r="K17" s="138"/>
-      <c r="L17" s="80"/>
-      <c r="M17" s="76" t="s">
+      <c r="J17" s="68"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="90" t="s">
         <v>170</v>
       </c>
-      <c r="N17" s="77">
+      <c r="N17" s="91">
         <f>SUM(N14:N16)</f>
         <v>86</v>
       </c>
-      <c r="O17" s="55"/>
-      <c r="P17" s="138"/>
-      <c r="Q17" s="7" t="s">
+      <c r="O17" s="69"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="R17" s="66" t="s">
+      <c r="R17" s="80" t="s">
         <v>172</v>
       </c>
-      <c r="S17" s="67">
+      <c r="S17" s="81">
         <v>18</v>
       </c>
-      <c r="T17" s="74" t="s">
+      <c r="T17" s="88" t="s">
         <v>173</v>
       </c>
-      <c r="U17" s="59"/>
-      <c r="V17" s="137"/>
-      <c r="W17" s="7" t="s">
+      <c r="U17" s="73"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="X17" s="66" t="s">
+      <c r="X17" s="80" t="s">
         <v>175</v>
       </c>
-      <c r="Y17" s="105">
+      <c r="Y17" s="119">
         <v>24</v>
       </c>
-      <c r="Z17" s="102" t="s">
+      <c r="Z17" s="116" t="s">
         <v>162</v>
       </c>
-      <c r="AA17" s="59"/>
+      <c r="AA17" s="73"/>
       <c r="AB17" s="164" t="s">
         <v>26</v>
       </c>
-      <c r="AC17" s="51" t="s">
+      <c r="AC17" s="65" t="s">
         <v>176</v>
       </c>
-      <c r="AD17" s="66" t="s">
+      <c r="AD17" s="80" t="s">
         <v>177</v>
       </c>
-      <c r="AE17" s="9">
+      <c r="AE17" s="23">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="152"/>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="95" t="s">
         <v>178</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="79">
         <v>14</v>
       </c>
-      <c r="E18" s="50"/>
+      <c r="E18" s="64"/>
       <c r="F18" s="163"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="90" t="s">
+      <c r="G18" s="103"/>
+      <c r="H18" s="104" t="s">
         <v>180</v>
       </c>
-      <c r="I18" s="91">
+      <c r="I18" s="105">
         <f>SUM(I15:I17)</f>
         <v>70</v>
       </c>
-      <c r="J18" s="54"/>
+      <c r="J18" s="68"/>
       <c r="K18" s="165" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="92" t="s">
+      <c r="L18" s="106" t="s">
         <v>181</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="N18" s="106">
+      <c r="N18" s="120">
         <v>21</v>
       </c>
-      <c r="O18" s="55"/>
-      <c r="P18" s="138"/>
-      <c r="Q18" s="7" t="s">
+      <c r="O18" s="69"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="R18" s="11" t="s">
+      <c r="R18" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="S18" s="67">
+      <c r="S18" s="81">
         <v>16</v>
       </c>
-      <c r="T18" s="107" t="s">
+      <c r="T18" s="121" t="s">
         <v>185</v>
       </c>
-      <c r="U18" s="59"/>
-      <c r="V18" s="137"/>
-      <c r="W18" s="80"/>
-      <c r="X18" s="76" t="s">
+      <c r="U18" s="73"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="94"/>
+      <c r="X18" s="90" t="s">
         <v>186</v>
       </c>
-      <c r="Y18" s="77">
+      <c r="Y18" s="91">
         <f>SUM(Y14:Y17)</f>
         <v>84</v>
       </c>
-      <c r="Z18" s="108"/>
-      <c r="AA18" s="109"/>
+      <c r="Z18" s="122"/>
+      <c r="AA18" s="123"/>
       <c r="AB18" s="164"/>
-      <c r="AC18" s="51" t="s">
+      <c r="AC18" s="65" t="s">
         <v>187</v>
       </c>
-      <c r="AD18" s="66" t="s">
+      <c r="AD18" s="80" t="s">
         <v>188</v>
       </c>
-      <c r="AE18" s="9">
+      <c r="AE18" s="23">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="152"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="86" t="s">
+      <c r="B19" s="69"/>
+      <c r="C19" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="D19" s="87">
+      <c r="D19" s="101">
         <f>SUM(D15:D18)</f>
         <v>70</v>
       </c>
-      <c r="E19" s="50"/>
-      <c r="F19" s="138" t="s">
+      <c r="E19" s="64"/>
+      <c r="F19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="I19" s="49">
+      <c r="I19" s="63">
         <v>14</v>
       </c>
-      <c r="J19" s="54"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="165"/>
-      <c r="L19" s="7" t="s">
+      <c r="L19" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="M19" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19" s="23">
         <v>39</v>
       </c>
-      <c r="O19" s="110"/>
-      <c r="P19" s="138"/>
-      <c r="Q19" s="7" t="s">
+      <c r="O19" s="124"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="R19" s="66" t="s">
+      <c r="R19" s="80" t="s">
         <v>195</v>
       </c>
-      <c r="S19" s="67">
+      <c r="S19" s="81">
         <v>18</v>
       </c>
-      <c r="T19" s="81" t="s">
+      <c r="T19" s="95" t="s">
         <v>196</v>
       </c>
-      <c r="U19" s="59"/>
-      <c r="V19" s="138" t="s">
+      <c r="U19" s="73"/>
+      <c r="V19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="W19" s="7" t="s">
+      <c r="W19" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="X19" s="70" t="s">
+      <c r="X19" s="84" t="s">
         <v>198</v>
       </c>
-      <c r="Y19" s="68">
+      <c r="Y19" s="82">
         <v>18</v>
       </c>
-      <c r="Z19" s="96"/>
-      <c r="AA19" s="59"/>
+      <c r="Z19" s="110"/>
+      <c r="AA19" s="73"/>
       <c r="AB19" s="164"/>
-      <c r="AC19" s="76"/>
-      <c r="AD19" s="77" t="s">
+      <c r="AC19" s="90"/>
+      <c r="AD19" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="AE19" s="78">
+      <c r="AE19" s="92">
         <f>SUM(AE17:AE18)</f>
         <v>54</v>
       </c>
@@ -3888,362 +3951,362 @@
       <c r="A20" s="166" t="s">
         <v>200</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="63">
         <v>14</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="31" t="s">
+      <c r="E20" s="64"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="I20" s="65">
+      <c r="I20" s="79">
         <v>39</v>
       </c>
-      <c r="J20" s="54"/>
+      <c r="J20" s="68"/>
       <c r="K20" s="165"/>
-      <c r="L20" s="80"/>
-      <c r="M20" s="76" t="s">
+      <c r="L20" s="94"/>
+      <c r="M20" s="90" t="s">
         <v>205</v>
       </c>
-      <c r="N20" s="77">
+      <c r="N20" s="91">
         <f>SUM(N18:N19)</f>
         <v>60</v>
       </c>
-      <c r="O20" s="110"/>
-      <c r="P20" s="138"/>
-      <c r="Q20" s="80"/>
-      <c r="R20" s="76" t="s">
+      <c r="O20" s="124"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="94"/>
+      <c r="R20" s="90" t="s">
         <v>206</v>
       </c>
-      <c r="S20" s="77">
+      <c r="S20" s="91">
         <f>SUM(S15:S19)</f>
         <v>86</v>
       </c>
-      <c r="T20" s="111"/>
-      <c r="U20" s="59"/>
-      <c r="V20" s="138"/>
-      <c r="W20" s="7" t="s">
+      <c r="T20" s="125"/>
+      <c r="U20" s="73"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="X20" s="70" t="s">
+      <c r="X20" s="84" t="s">
         <v>208</v>
       </c>
-      <c r="Y20" s="68">
+      <c r="Y20" s="82">
         <v>18</v>
       </c>
-      <c r="Z20" s="102"/>
-      <c r="AA20" s="59"/>
+      <c r="Z20" s="116"/>
+      <c r="AA20" s="73"/>
     </row>
     <row r="21" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="166"/>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="D21" s="65">
+      <c r="D21" s="79">
         <v>39</v>
       </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="76" t="s">
+      <c r="E21" s="64"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="90" t="s">
         <v>211</v>
       </c>
-      <c r="I21" s="77">
+      <c r="I21" s="91">
         <f>SUM(I19:I20)</f>
         <v>53</v>
       </c>
-      <c r="J21" s="54"/>
-      <c r="K21" s="45"/>
-      <c r="O21" s="110"/>
-      <c r="P21" s="138" t="s">
+      <c r="J21" s="68"/>
+      <c r="K21" s="59"/>
+      <c r="O21" s="124"/>
+      <c r="P21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="15" t="s">
+      <c r="Q21" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="R21" s="112" t="s">
+      <c r="R21" s="126" t="s">
         <v>213</v>
       </c>
-      <c r="S21" s="99">
+      <c r="S21" s="113">
         <v>50</v>
       </c>
-      <c r="T21" s="113" t="s">
+      <c r="T21" s="127" t="s">
         <v>214</v>
       </c>
-      <c r="U21" s="109"/>
-      <c r="V21" s="138"/>
-      <c r="W21" s="114" t="s">
+      <c r="U21" s="123"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="X21" s="66" t="s">
+      <c r="X21" s="80" t="s">
         <v>216</v>
       </c>
-      <c r="Y21" s="68">
+      <c r="Y21" s="82">
         <v>45</v>
       </c>
-      <c r="Z21" s="100"/>
-      <c r="AB21" s="115"/>
+      <c r="Z21" s="114"/>
+      <c r="AB21" s="129"/>
     </row>
     <row r="22" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="166"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="76" t="s">
+      <c r="B22" s="94"/>
+      <c r="C22" s="90" t="s">
         <v>217</v>
       </c>
-      <c r="D22" s="77">
+      <c r="D22" s="91">
         <f>SUM(D20:D21)</f>
         <v>53</v>
       </c>
-      <c r="E22" s="50"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="117"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="115"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="118"/>
-      <c r="O22" s="110"/>
-      <c r="P22" s="138"/>
-      <c r="Q22" s="80"/>
-      <c r="R22" s="76" t="s">
+      <c r="E22" s="64"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="131"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="129"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="132"/>
+      <c r="O22" s="124"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="94"/>
+      <c r="R22" s="90" t="s">
         <v>218</v>
       </c>
-      <c r="S22" s="77">
+      <c r="S22" s="91">
         <f ca="1">SUM(S21:S25)</f>
         <v>50</v>
       </c>
-      <c r="T22" s="119"/>
-      <c r="U22" s="109"/>
-      <c r="V22" s="138"/>
-      <c r="W22" s="76"/>
-      <c r="X22" s="77" t="s">
+      <c r="T22" s="133"/>
+      <c r="U22" s="123"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="90"/>
+      <c r="X22" s="91" t="s">
         <v>219</v>
       </c>
-      <c r="Y22" s="77">
+      <c r="Y22" s="91">
         <f ca="1">SUM(Y19:Y25)</f>
         <v>81</v>
       </c>
-      <c r="Z22" s="120"/>
-      <c r="AA22" s="59"/>
-      <c r="AB22" s="115"/>
+      <c r="Z22" s="134"/>
+      <c r="AA22" s="73"/>
+      <c r="AB22" s="129"/>
     </row>
     <row r="23" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="121"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="115"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="117"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="118"/>
-      <c r="O23" s="110"/>
-      <c r="P23" s="122"/>
-      <c r="Q23" s="123"/>
-      <c r="R23" s="123"/>
-      <c r="S23" s="123"/>
-      <c r="T23" s="59"/>
-      <c r="U23" s="109"/>
-      <c r="V23" s="115"/>
-      <c r="W23" s="123"/>
-      <c r="X23" s="123"/>
-      <c r="Y23" s="123"/>
-      <c r="Z23" s="124"/>
-      <c r="AA23" s="124"/>
-      <c r="AB23" s="115"/>
+      <c r="A23" s="135"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="131"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="132"/>
+      <c r="O23" s="124"/>
+      <c r="P23" s="136"/>
+      <c r="Q23" s="137"/>
+      <c r="R23" s="137"/>
+      <c r="S23" s="137"/>
+      <c r="T23" s="73"/>
+      <c r="U23" s="123"/>
+      <c r="V23" s="129"/>
+      <c r="W23" s="137"/>
+      <c r="X23" s="137"/>
+      <c r="Y23" s="137"/>
+      <c r="Z23" s="138"/>
+      <c r="AA23" s="138"/>
+      <c r="AB23" s="129"/>
     </row>
     <row r="24" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="121"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="115"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="118"/>
-      <c r="O24" s="110"/>
-      <c r="P24" s="122"/>
-      <c r="R24" s="123"/>
-      <c r="S24" s="123"/>
-      <c r="T24" s="125"/>
-      <c r="U24" s="109"/>
-      <c r="V24" s="115"/>
-      <c r="W24" s="123"/>
-      <c r="X24" s="123"/>
-      <c r="Y24" s="123"/>
-      <c r="Z24" s="124"/>
-      <c r="AA24" s="124"/>
-      <c r="AB24" s="115"/>
+      <c r="A24" s="135"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="130"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="131"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="132"/>
+      <c r="O24" s="124"/>
+      <c r="P24" s="136"/>
+      <c r="R24" s="137"/>
+      <c r="S24" s="137"/>
+      <c r="T24" s="139"/>
+      <c r="U24" s="123"/>
+      <c r="V24" s="129"/>
+      <c r="W24" s="137"/>
+      <c r="X24" s="137"/>
+      <c r="Y24" s="137"/>
+      <c r="Z24" s="138"/>
+      <c r="AA24" s="138"/>
+      <c r="AB24" s="129"/>
     </row>
     <row r="25" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="126"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="115"/>
-      <c r="G25" s="116"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="117"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="118"/>
-      <c r="O25" s="110"/>
-      <c r="P25" s="122"/>
-      <c r="Q25" s="123"/>
-      <c r="R25" s="123"/>
-      <c r="S25" s="123"/>
-      <c r="T25" s="125"/>
-      <c r="U25" s="109"/>
-      <c r="V25" s="115"/>
-      <c r="W25" s="123"/>
-      <c r="X25" s="123"/>
-      <c r="Y25" s="123"/>
-      <c r="Z25" s="124"/>
-      <c r="AA25" s="124"/>
-      <c r="AB25" s="115"/>
+      <c r="A25" s="140"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="129"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="131"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="132"/>
+      <c r="O25" s="124"/>
+      <c r="P25" s="136"/>
+      <c r="Q25" s="137"/>
+      <c r="R25" s="137"/>
+      <c r="S25" s="137"/>
+      <c r="T25" s="139"/>
+      <c r="U25" s="123"/>
+      <c r="V25" s="129"/>
+      <c r="W25" s="137"/>
+      <c r="X25" s="137"/>
+      <c r="Y25" s="137"/>
+      <c r="Z25" s="138"/>
+      <c r="AA25" s="138"/>
+      <c r="AB25" s="129"/>
     </row>
     <row r="26" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="126"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="115"/>
-      <c r="J26" s="45"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="122"/>
-      <c r="U26" s="127"/>
-      <c r="AB26" s="115"/>
+      <c r="A26" s="140"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="129"/>
+      <c r="J26" s="59"/>
+      <c r="O26" s="69"/>
+      <c r="P26" s="136"/>
+      <c r="U26" s="141"/>
+      <c r="AB26" s="129"/>
     </row>
     <row r="27" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="126"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="115"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="118"/>
-      <c r="O27" s="55"/>
-      <c r="P27" s="122"/>
-      <c r="U27" s="127"/>
-      <c r="AB27" s="115"/>
+      <c r="A27" s="140"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="129"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="132"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="136"/>
+      <c r="U27" s="141"/>
+      <c r="AB27" s="129"/>
     </row>
     <row r="28" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="128"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="115"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="118"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="122"/>
-      <c r="U28" s="59"/>
-      <c r="AB28" s="115"/>
+      <c r="A28" s="142"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="129"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="132"/>
+      <c r="O28" s="69"/>
+      <c r="P28" s="136"/>
+      <c r="U28" s="73"/>
+      <c r="AB28" s="129"/>
     </row>
     <row r="29" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E29" s="50"/>
-      <c r="F29" s="115"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="118"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="122"/>
-      <c r="U29" s="59"/>
-      <c r="AB29" s="115"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="129"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="132"/>
+      <c r="O29" s="69"/>
+      <c r="P29" s="136"/>
+      <c r="U29" s="73"/>
+      <c r="AB29" s="129"/>
     </row>
     <row r="30" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="50"/>
-      <c r="F30" s="115"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="118"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="122"/>
-      <c r="U30" s="59"/>
-      <c r="AB30" s="129"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="129"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="132"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="136"/>
+      <c r="U30" s="73"/>
+      <c r="AB30" s="143"/>
     </row>
     <row r="31" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E31" s="50"/>
-      <c r="F31" s="115"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="118"/>
-      <c r="O31" s="55"/>
-      <c r="P31" s="122"/>
-      <c r="U31" s="59"/>
-      <c r="AB31" s="129"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="129"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="132"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="136"/>
+      <c r="U31" s="73"/>
+      <c r="AB31" s="143"/>
     </row>
     <row r="32" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E32" s="50"/>
-      <c r="F32" s="129"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="118"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="129"/>
-      <c r="U32" s="124"/>
-      <c r="AB32" s="129"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="143"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="132"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="143"/>
+      <c r="U32" s="138"/>
+      <c r="AB32" s="143"/>
     </row>
     <row r="33" spans="5:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E33" s="50"/>
-      <c r="F33" s="129"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="118"/>
-      <c r="O33" s="55"/>
-      <c r="P33" s="129"/>
-      <c r="U33" s="124"/>
-      <c r="AB33" s="48"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="143"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="132"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="143"/>
+      <c r="U33" s="138"/>
+      <c r="AB33" s="62"/>
     </row>
     <row r="34" spans="5:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E34" s="50"/>
-      <c r="F34" s="129"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="118"/>
-      <c r="O34" s="55"/>
-      <c r="P34" s="129"/>
-      <c r="U34" s="124"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="143"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="132"/>
+      <c r="O34" s="69"/>
+      <c r="P34" s="143"/>
+      <c r="U34" s="138"/>
     </row>
     <row r="35" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E35" s="50"/>
-      <c r="F35" s="128"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="47"/>
-      <c r="O35" s="110"/>
-      <c r="P35" s="48"/>
-      <c r="U35" s="124"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="142"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="61"/>
+      <c r="O35" s="124"/>
+      <c r="P35" s="62"/>
+      <c r="U35" s="138"/>
     </row>
     <row r="36" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E36" s="50"/>
-      <c r="J36" s="54"/>
-      <c r="O36" s="110"/>
-      <c r="U36" s="124"/>
+      <c r="E36" s="64"/>
+      <c r="J36" s="68"/>
+      <c r="O36" s="124"/>
+      <c r="U36" s="138"/>
     </row>
     <row r="37" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E37" s="88"/>
-      <c r="J37" s="45"/>
-      <c r="O37" s="110"/>
-      <c r="U37" s="130"/>
+      <c r="E37" s="102"/>
+      <c r="J37" s="59"/>
+      <c r="O37" s="124"/>
+      <c r="U37" s="144"/>
     </row>
     <row r="38" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E38" s="88"/>
-      <c r="J38" s="45"/>
-      <c r="O38" s="110"/>
-      <c r="U38" s="130"/>
+      <c r="E38" s="102"/>
+      <c r="J38" s="59"/>
+      <c r="O38" s="124"/>
+      <c r="U38" s="144"/>
     </row>
     <row r="39" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E39" s="88"/>
-      <c r="J39" s="45"/>
-      <c r="O39" s="48"/>
-      <c r="U39" s="130"/>
+      <c r="E39" s="102"/>
+      <c r="J39" s="59"/>
+      <c r="O39" s="62"/>
+      <c r="U39" s="144"/>
     </row>
     <row r="40" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E40" s="88"/>
-      <c r="J40" s="45"/>
-      <c r="U40" s="130"/>
+      <c r="E40" s="102"/>
+      <c r="J40" s="59"/>
+      <c r="U40" s="144"/>
     </row>
     <row r="41" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E41" s="46"/>
-      <c r="J41" s="47"/>
-      <c r="U41" s="131"/>
+      <c r="E41" s="60"/>
+      <c r="J41" s="61"/>
+      <c r="U41" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -4299,140 +4362,293 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ15"/>
+  <dimension ref="A1:AMJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="132" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="132" customWidth="1"/>
-    <col min="3" max="1024" width="14.42578125" style="132"/>
+    <col min="1" max="1" width="25.28515625" style="146" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="146" customWidth="1"/>
+    <col min="3" max="1024" width="14.42578125" style="146"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="147" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="134" t="s">
+      <c r="B1" s="148" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="149" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="136">
+      <c r="B2" s="150">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="135" t="s">
+      <c r="A3" s="149" t="s">
         <v>223</v>
       </c>
-      <c r="B3" s="136">
+      <c r="B3" s="150">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="149" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="149" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="149" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="149" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="149" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="149" t="s">
         <v>230</v>
       </c>
-      <c r="B4">
+      <c r="B10" s="150">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="149" t="s">
         <v>231</v>
       </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B11" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="B8">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>226</v>
-      </c>
-      <c r="B9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B12" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="149" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="149" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="149" t="s">
         <v>235</v>
       </c>
-      <c r="B10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>233</v>
-      </c>
-      <c r="B11">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>227</v>
-      </c>
-      <c r="B12">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>228</v>
-      </c>
-      <c r="B13">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>229</v>
-      </c>
-      <c r="B14">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>234</v>
-      </c>
-      <c r="B15">
-        <v>24</v>
+      <c r="B15" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="149" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="149" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="149" t="s">
+        <v>238</v>
+      </c>
+      <c r="B18" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="149" t="s">
+        <v>239</v>
+      </c>
+      <c r="B19" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="149" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="149" t="s">
+        <v>241</v>
+      </c>
+      <c r="B21" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="149" t="s">
+        <v>242</v>
+      </c>
+      <c r="B22" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="149" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="149" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="B25" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="B27" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="149" t="s">
+        <v>248</v>
+      </c>
+      <c r="B28" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="149" t="s">
+        <v>249</v>
+      </c>
+      <c r="B29" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="149" t="s">
+        <v>250</v>
+      </c>
+      <c r="B30" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="149" t="s">
+        <v>251</v>
+      </c>
+      <c r="B31" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="149" t="s">
+        <v>252</v>
+      </c>
+      <c r="B32" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="149" t="s">
+        <v>253</v>
+      </c>
+      <c r="B33" s="150">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="149" t="s">
+        <v>254</v>
+      </c>
+      <c r="B34" s="150">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Revert "Updated warnings for having too many students and not selecting a semester""
</commit_message>
<xml_diff>
--- a/SCE_ProgramsCourses (copy).xlsx
+++ b/SCE_ProgramsCourses (copy).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\2023-01_Team6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBC2D38-02B5-45D1-A17E-958487C3A544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC72B3C-B7BD-4FA9-BE56-0B034A9C5D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="3270" windowWidth="21600" windowHeight="10140" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Core Courses (PCOM)" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
   <si>
     <t>Color Code</t>
   </si>
@@ -866,82 +866,25 @@
     <t>11-539</t>
   </si>
   <si>
-    <t>11-540</t>
-  </si>
-  <si>
-    <t>11-541</t>
-  </si>
-  <si>
-    <t>11-542</t>
-  </si>
-  <si>
-    <t>11-543</t>
-  </si>
-  <si>
-    <t>11-544</t>
-  </si>
-  <si>
-    <t>11-545</t>
-  </si>
-  <si>
-    <t>11-546</t>
-  </si>
-  <si>
-    <t>11-547</t>
-  </si>
-  <si>
-    <t>11-548</t>
-  </si>
-  <si>
-    <t>11-549</t>
-  </si>
-  <si>
-    <t>11-550</t>
-  </si>
-  <si>
-    <t>11-551</t>
-  </si>
-  <si>
-    <t>11-552</t>
-  </si>
-  <si>
-    <t>11-553</t>
-  </si>
-  <si>
-    <t>11-554</t>
-  </si>
-  <si>
-    <t>11-555</t>
-  </si>
-  <si>
-    <t>11-556</t>
-  </si>
-  <si>
-    <t>11-557</t>
-  </si>
-  <si>
-    <t>11-558</t>
-  </si>
-  <si>
-    <t>11-559</t>
-  </si>
-  <si>
-    <t>11-560</t>
-  </si>
-  <si>
-    <t>11-561 Lab</t>
-  </si>
-  <si>
-    <t>11-562 Lab</t>
-  </si>
-  <si>
-    <t>11-563 Lab</t>
-  </si>
-  <si>
-    <t>11-564 Lab</t>
-  </si>
-  <si>
-    <t>11-565 Lab</t>
+    <t>11-5310</t>
+  </si>
+  <si>
+    <t>11-323C Computer Lab</t>
+  </si>
+  <si>
+    <t>11-324C Computer Lab</t>
+  </si>
+  <si>
+    <t>11-325C Computer Lab</t>
+  </si>
+  <si>
+    <t>11-625C Computer Lab</t>
+  </si>
+  <si>
+    <t>11-5312</t>
+  </si>
+  <si>
+    <t>11-329C Computer Lab</t>
   </si>
 </sst>
 </file>
@@ -954,7 +897,7 @@
     <numFmt numFmtId="166" formatCode="\$#,##0.00_);[Red]&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="167" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1054,12 +997,6 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1549,53 +1486,11 @@
   </cellStyleXfs>
   <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1984,6 +1879,48 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2431,211 +2368,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="141"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="142" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="17" t="s">
+      <c r="B6" s="142"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="6">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="137"/>
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="9">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="137"/>
+      <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="9">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="137"/>
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="24" t="s">
+      <c r="A11" s="137"/>
+      <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="27" t="s">
+      <c r="A12" s="137"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="14">
         <f>SUM(D7:D11)</f>
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="6">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="30" t="s">
+      <c r="A14" s="137"/>
+      <c r="B14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="18">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="137"/>
+      <c r="B15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="9">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34" t="s">
+      <c r="A16" s="137"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="21">
         <f>SUM(D13:D15)</f>
         <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="37">
+      <c r="D17" s="23">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="21" t="s">
+      <c r="A18" s="138"/>
+      <c r="B18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="9">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="38" t="s">
+      <c r="A19" s="138"/>
+      <c r="B19" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="9">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41" t="s">
+      <c r="A20" s="138"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="28">
         <f>SUM(D17:D19)</f>
         <v>82</v>
       </c>
@@ -2672,295 +2609,295 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="141"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="17" t="s">
+      <c r="B6" s="142"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="6">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="137"/>
+      <c r="B8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="137"/>
+      <c r="B9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="9">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="43" t="s">
+      <c r="A10" s="137"/>
+      <c r="B10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="9">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="137"/>
+      <c r="B11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="137"/>
+      <c r="B12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27" t="s">
+      <c r="A13" s="137"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="14">
         <f>SUM(D7:D12)</f>
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="143"/>
+      <c r="B15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="21" t="s">
+      <c r="A16" s="143"/>
+      <c r="B16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="143"/>
+      <c r="B17" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="43" t="s">
+      <c r="A18" s="143"/>
+      <c r="B18" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="143"/>
+      <c r="B19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="9">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="27" t="s">
+      <c r="A20" s="143"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="14">
         <f>SUM(D14:D19)</f>
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="23">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="48" t="s">
+      <c r="A22" s="143"/>
+      <c r="B22" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="50">
+      <c r="D22" s="36">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="48" t="s">
+      <c r="A23" s="143"/>
+      <c r="B23" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="50">
+      <c r="D23" s="36">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="48" t="s">
+      <c r="A24" s="143"/>
+      <c r="B24" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="50">
+      <c r="D24" s="36">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="48" t="s">
+      <c r="A25" s="143"/>
+      <c r="B25" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="51" t="s">
+      <c r="A26" s="143"/>
+      <c r="B26" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="53">
+      <c r="D26" s="39">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="55" t="s">
+      <c r="A27" s="143"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="56">
+      <c r="D27" s="42">
         <f>SUM(D21:D26)</f>
         <v>76</v>
       </c>
@@ -2990,186 +2927,186 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="57" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="57" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" style="57" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="57" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="57" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="57" customWidth="1"/>
-    <col min="8" max="8" width="38.42578125" style="57" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="57" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="57" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="57" customWidth="1"/>
-    <col min="13" max="13" width="39.42578125" style="57" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="57" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" style="57" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="57" customWidth="1"/>
-    <col min="18" max="18" width="43" style="57" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="57" customWidth="1"/>
-    <col min="20" max="20" width="58.42578125" style="57" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="57" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" style="57" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" style="57" customWidth="1"/>
-    <col min="24" max="24" width="26.5703125" style="57" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" style="57" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" style="57" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" style="57" customWidth="1"/>
-    <col min="28" max="28" width="7.5703125" style="57" customWidth="1"/>
-    <col min="29" max="29" width="8.85546875" style="57" customWidth="1"/>
-    <col min="30" max="30" width="39.85546875" style="57" customWidth="1"/>
-    <col min="31" max="31" width="13.5703125" style="57" customWidth="1"/>
-    <col min="32" max="1024" width="9.42578125" style="57"/>
+    <col min="1" max="1" width="7.5703125" style="43" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="43" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" style="43" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="43" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="43" customWidth="1"/>
+    <col min="8" max="8" width="38.42578125" style="43" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="43" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="43" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="43" customWidth="1"/>
+    <col min="13" max="13" width="39.42578125" style="43" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="43" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" style="43" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="43" customWidth="1"/>
+    <col min="18" max="18" width="43" style="43" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="43" customWidth="1"/>
+    <col min="20" max="20" width="58.42578125" style="43" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="43" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" style="43" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" style="43" customWidth="1"/>
+    <col min="24" max="24" width="26.5703125" style="43" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="43" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" style="43" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="43" customWidth="1"/>
+    <col min="28" max="28" width="7.5703125" style="43" customWidth="1"/>
+    <col min="29" max="29" width="8.85546875" style="43" customWidth="1"/>
+    <col min="30" max="30" width="39.85546875" style="43" customWidth="1"/>
+    <col min="31" max="31" width="13.5703125" style="43" customWidth="1"/>
+    <col min="32" max="1024" width="9.42578125" style="43"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="145"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
+      <c r="A5" s="45"/>
     </row>
     <row r="6" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="142" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="142"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="146" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="46"/>
+      <c r="F6" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="3" t="s">
+      <c r="G6" s="147"/>
+      <c r="H6" s="147"/>
+      <c r="I6" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="61"/>
-      <c r="K6" s="4" t="s">
+      <c r="J6" s="47"/>
+      <c r="K6" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="3" t="s">
+      <c r="L6" s="147"/>
+      <c r="M6" s="147"/>
+      <c r="N6" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="62"/>
-      <c r="P6" s="4" t="s">
+      <c r="O6" s="48"/>
+      <c r="P6" s="147" t="s">
         <v>74</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="3" t="s">
+      <c r="Q6" s="147"/>
+      <c r="R6" s="147"/>
+      <c r="S6" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="149" t="s">
         <v>75</v>
       </c>
-      <c r="V6" s="4" t="s">
+      <c r="V6" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="1" t="s">
+      <c r="W6" s="147"/>
+      <c r="X6" s="147"/>
+      <c r="Y6" s="150" t="s">
         <v>5</v>
       </c>
       <c r="Z6" s="151" t="s">
         <v>75</v>
       </c>
-      <c r="AB6" s="11" t="s">
+      <c r="AB6" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="5" t="s">
+      <c r="AC6" s="142"/>
+      <c r="AD6" s="142"/>
+      <c r="AE6" s="146" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="2"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="1"/>
+      <c r="A7" s="142"/>
+      <c r="B7" s="142"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="147"/>
+      <c r="M7" s="147"/>
+      <c r="N7" s="148"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="147"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="147"/>
+      <c r="S7" s="148"/>
+      <c r="T7" s="149"/>
+      <c r="V7" s="147"/>
+      <c r="W7" s="147"/>
+      <c r="X7" s="147"/>
+      <c r="Y7" s="150"/>
       <c r="Z7" s="151"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="5"/>
+      <c r="AB7" s="142"/>
+      <c r="AC7" s="142"/>
+      <c r="AD7" s="142"/>
+      <c r="AE7" s="146"/>
     </row>
     <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="2"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="1"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="146"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="148"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="147"/>
+      <c r="L8" s="147"/>
+      <c r="M8" s="147"/>
+      <c r="N8" s="148"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="147"/>
+      <c r="Q8" s="147"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="148"/>
+      <c r="T8" s="149"/>
+      <c r="V8" s="147"/>
+      <c r="W8" s="147"/>
+      <c r="X8" s="147"/>
+      <c r="Y8" s="150"/>
       <c r="Z8" s="151"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="5"/>
+      <c r="AB8" s="142"/>
+      <c r="AC8" s="142"/>
+      <c r="AD8" s="142"/>
+      <c r="AE8" s="146"/>
     </row>
     <row r="9" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="152" t="s">
@@ -3184,65 +3121,65 @@
       <c r="D9" s="155">
         <v>21</v>
       </c>
-      <c r="E9" s="64"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="156" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="66" t="s">
+      <c r="H9" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="67">
+      <c r="I9" s="53">
         <v>21</v>
       </c>
-      <c r="J9" s="68"/>
-      <c r="K9" s="9" t="s">
+      <c r="J9" s="54"/>
+      <c r="K9" s="138" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="6">
         <v>21</v>
       </c>
-      <c r="O9" s="69"/>
+      <c r="O9" s="55"/>
       <c r="P9" s="157" t="s">
         <v>78</v>
       </c>
-      <c r="Q9" s="65" t="s">
+      <c r="Q9" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="R9" s="70" t="s">
+      <c r="R9" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="S9" s="71">
+      <c r="S9" s="57">
         <v>16</v>
       </c>
-      <c r="T9" s="72"/>
-      <c r="U9" s="73"/>
-      <c r="V9" s="9" t="s">
+      <c r="T9" s="58"/>
+      <c r="U9" s="59"/>
+      <c r="V9" s="138" t="s">
         <v>78</v>
       </c>
-      <c r="W9" s="74"/>
-      <c r="X9" s="74"/>
-      <c r="Y9" s="74"/>
-      <c r="Z9" s="75"/>
-      <c r="AA9" s="76"/>
-      <c r="AB9" s="9" t="s">
+      <c r="W9" s="60"/>
+      <c r="X9" s="60"/>
+      <c r="Y9" s="60"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="138" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="18" t="s">
+      <c r="AC9" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="AD9" s="77" t="s">
+      <c r="AD9" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="AE9" s="78">
+      <c r="AE9" s="64">
         <v>18</v>
       </c>
     </row>
@@ -3251,61 +3188,61 @@
       <c r="B10" s="153"/>
       <c r="C10" s="154"/>
       <c r="D10" s="155"/>
-      <c r="E10" s="64"/>
+      <c r="E10" s="50"/>
       <c r="F10" s="156"/>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="H10" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="I10" s="79">
+      <c r="I10" s="65">
         <v>14</v>
       </c>
-      <c r="J10" s="68"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="21" t="s">
+      <c r="J10" s="54"/>
+      <c r="K10" s="138"/>
+      <c r="L10" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="9">
         <v>21</v>
       </c>
-      <c r="O10" s="69"/>
+      <c r="O10" s="55"/>
       <c r="P10" s="157"/>
-      <c r="Q10" s="21" t="s">
+      <c r="Q10" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="R10" s="80" t="s">
+      <c r="R10" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="S10" s="81">
+      <c r="S10" s="67">
         <v>16</v>
       </c>
-      <c r="T10" s="72"/>
-      <c r="U10" s="73"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="21" t="s">
+      <c r="T10" s="58"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="138"/>
+      <c r="W10" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="X10" s="80" t="s">
+      <c r="X10" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="Y10" s="82">
+      <c r="Y10" s="68">
         <v>18</v>
       </c>
-      <c r="Z10" s="83"/>
-      <c r="AA10" s="76"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="21" t="s">
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="138"/>
+      <c r="AC10" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="AD10" s="84" t="s">
+      <c r="AD10" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="AE10" s="85">
+      <c r="AE10" s="71">
         <v>12</v>
       </c>
     </row>
@@ -3320,7 +3257,7 @@
       <c r="D11" s="160">
         <v>14</v>
       </c>
-      <c r="E11" s="87"/>
+      <c r="E11" s="73"/>
       <c r="F11" s="156"/>
       <c r="G11" s="161" t="s">
         <v>101</v>
@@ -3331,52 +3268,52 @@
       <c r="I11" s="160">
         <v>21</v>
       </c>
-      <c r="J11" s="68"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="21" t="s">
+      <c r="J11" s="54"/>
+      <c r="K11" s="138"/>
+      <c r="L11" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="M11" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="9">
         <v>15</v>
       </c>
-      <c r="O11" s="69"/>
+      <c r="O11" s="55"/>
       <c r="P11" s="157"/>
-      <c r="Q11" s="21" t="s">
+      <c r="Q11" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="R11" s="80" t="s">
+      <c r="R11" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="S11" s="81">
+      <c r="S11" s="67">
         <v>16</v>
       </c>
-      <c r="T11" s="88" t="s">
+      <c r="T11" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="U11" s="73"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="21" t="s">
+      <c r="U11" s="59"/>
+      <c r="V11" s="138"/>
+      <c r="W11" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="X11" s="80" t="s">
+      <c r="X11" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="Y11" s="82">
+      <c r="Y11" s="68">
         <v>24</v>
       </c>
-      <c r="Z11" s="83"/>
-      <c r="AA11" s="76"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="21" t="s">
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="138"/>
+      <c r="AC11" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AD11" s="84" t="s">
+      <c r="AD11" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="AE11" s="85">
+      <c r="AE11" s="71">
         <v>12</v>
       </c>
     </row>
@@ -3385,199 +3322,199 @@
       <c r="B12" s="158"/>
       <c r="C12" s="159"/>
       <c r="D12" s="160"/>
-      <c r="E12" s="87"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="156"/>
       <c r="G12" s="161"/>
       <c r="H12" s="159"/>
       <c r="I12" s="160"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="21" t="s">
+      <c r="J12" s="54"/>
+      <c r="K12" s="138"/>
+      <c r="L12" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="M12" s="89" t="s">
+      <c r="M12" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="9">
         <v>50</v>
       </c>
-      <c r="O12" s="69"/>
+      <c r="O12" s="55"/>
       <c r="P12" s="157"/>
-      <c r="Q12" s="21" t="s">
+      <c r="Q12" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="R12" s="80" t="s">
+      <c r="R12" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="S12" s="81">
+      <c r="S12" s="67">
         <v>16</v>
       </c>
-      <c r="T12" s="72" t="s">
+      <c r="T12" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="U12" s="73"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="21" t="s">
+      <c r="U12" s="59"/>
+      <c r="V12" s="138"/>
+      <c r="W12" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="X12" s="80" t="s">
+      <c r="X12" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="Y12" s="82">
+      <c r="Y12" s="68">
         <v>24</v>
       </c>
-      <c r="Z12" s="83" t="s">
+      <c r="Z12" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="AA12" s="76"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="90"/>
-      <c r="AD12" s="91" t="s">
+      <c r="AA12" s="62"/>
+      <c r="AB12" s="138"/>
+      <c r="AC12" s="76"/>
+      <c r="AD12" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="AE12" s="92">
+      <c r="AE12" s="78">
         <f>SUM(AE9:AE11)</f>
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="152"/>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="72" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="79">
+      <c r="D13" s="65">
         <v>21</v>
       </c>
-      <c r="E13" s="87"/>
+      <c r="E13" s="73"/>
       <c r="F13" s="156"/>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="H13" s="93" t="s">
+      <c r="H13" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="I13" s="79">
+      <c r="I13" s="65">
         <v>14</v>
       </c>
-      <c r="J13" s="68"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="90" t="s">
+      <c r="J13" s="54"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="N13" s="91">
+      <c r="N13" s="77">
         <f>SUM(N9:N12)</f>
         <v>107</v>
       </c>
-      <c r="O13" s="69"/>
+      <c r="O13" s="55"/>
       <c r="P13" s="157"/>
-      <c r="Q13" s="21" t="s">
+      <c r="Q13" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="R13" s="80" t="s">
+      <c r="R13" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="S13" s="81">
+      <c r="S13" s="67">
         <v>16</v>
       </c>
-      <c r="T13" s="95" t="s">
+      <c r="T13" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="U13" s="73"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="94"/>
-      <c r="X13" s="90" t="s">
+      <c r="U13" s="59"/>
+      <c r="V13" s="138"/>
+      <c r="W13" s="80"/>
+      <c r="X13" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="Y13" s="91">
+      <c r="Y13" s="77">
         <f>SUM(Y9:Y12)</f>
         <v>66</v>
       </c>
-      <c r="Z13" s="96"/>
-      <c r="AA13" s="97"/>
+      <c r="Z13" s="82"/>
+      <c r="AA13" s="83"/>
       <c r="AB13" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="AC13" s="65" t="s">
+      <c r="AC13" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="AD13" s="98" t="s">
+      <c r="AD13" s="84" t="s">
         <v>130</v>
       </c>
-      <c r="AE13" s="99">
+      <c r="AE13" s="85">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="152"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="100" t="s">
+      <c r="B14" s="55"/>
+      <c r="C14" s="86" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="101">
+      <c r="D14" s="87">
         <f>SUM(D9:D13)</f>
         <v>56</v>
       </c>
-      <c r="E14" s="102"/>
+      <c r="E14" s="88"/>
       <c r="F14" s="156"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="104" t="s">
+      <c r="G14" s="89"/>
+      <c r="H14" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="I14" s="105">
+      <c r="I14" s="91">
         <f>SUM(I9:I13)</f>
         <v>70</v>
       </c>
-      <c r="J14" s="68"/>
-      <c r="K14" s="9" t="s">
+      <c r="J14" s="54"/>
+      <c r="K14" s="138" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="M14" s="106" t="s">
+      <c r="M14" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="6">
         <v>15</v>
       </c>
-      <c r="O14" s="69"/>
+      <c r="O14" s="55"/>
       <c r="P14" s="157"/>
-      <c r="Q14" s="94"/>
-      <c r="R14" s="90" t="s">
+      <c r="Q14" s="80"/>
+      <c r="R14" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="S14" s="91">
+      <c r="S14" s="77">
         <f>SUM(S9:S13)</f>
         <v>80</v>
       </c>
-      <c r="T14" s="107"/>
-      <c r="U14" s="97"/>
-      <c r="V14" s="10" t="s">
+      <c r="T14" s="93"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="W14" s="18" t="s">
+      <c r="W14" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="X14" s="108" t="s">
+      <c r="X14" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="Y14" s="109">
+      <c r="Y14" s="95">
         <v>18</v>
       </c>
-      <c r="Z14" s="110"/>
-      <c r="AA14" s="73"/>
+      <c r="Z14" s="96"/>
+      <c r="AA14" s="59"/>
       <c r="AB14" s="162"/>
-      <c r="AC14" s="65" t="s">
+      <c r="AC14" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="AD14" s="80" t="s">
+      <c r="AD14" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="AE14" s="111">
+      <c r="AE14" s="97">
         <v>28</v>
       </c>
     </row>
@@ -3585,364 +3522,364 @@
       <c r="A15" s="152" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="112" t="s">
+      <c r="B15" s="98" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="49">
         <v>14</v>
       </c>
-      <c r="E15" s="64"/>
+      <c r="E15" s="50"/>
       <c r="F15" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="I15" s="63">
+      <c r="I15" s="49">
         <v>21</v>
       </c>
-      <c r="J15" s="68"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="21" t="s">
+      <c r="J15" s="54"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="M15" s="22" t="s">
+      <c r="M15" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="9">
         <v>21</v>
       </c>
-      <c r="O15" s="69"/>
-      <c r="P15" s="9" t="s">
+      <c r="O15" s="55"/>
+      <c r="P15" s="138" t="s">
         <v>18</v>
       </c>
-      <c r="Q15" s="18" t="s">
+      <c r="Q15" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="R15" s="108" t="s">
+      <c r="R15" s="94" t="s">
         <v>147</v>
       </c>
-      <c r="S15" s="113">
+      <c r="S15" s="99">
         <v>18</v>
       </c>
-      <c r="T15" s="72" t="s">
+      <c r="T15" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="U15" s="73"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="21" t="s">
+      <c r="U15" s="59"/>
+      <c r="V15" s="137"/>
+      <c r="W15" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="X15" s="80" t="s">
+      <c r="X15" s="66" t="s">
         <v>150</v>
       </c>
-      <c r="Y15" s="82">
+      <c r="Y15" s="68">
         <v>18</v>
       </c>
-      <c r="Z15" s="114"/>
+      <c r="Z15" s="100"/>
       <c r="AB15" s="162"/>
-      <c r="AC15" s="65" t="s">
+      <c r="AC15" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AD15" s="80" t="s">
+      <c r="AD15" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="AE15" s="81">
+      <c r="AE15" s="67">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="152"/>
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D16" s="115">
+      <c r="D16" s="101">
         <v>21</v>
       </c>
-      <c r="E16" s="64"/>
+      <c r="E16" s="50"/>
       <c r="F16" s="163"/>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="H16" s="45" t="s">
+      <c r="H16" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="I16" s="79">
+      <c r="I16" s="65">
         <v>14</v>
       </c>
-      <c r="J16" s="68"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="21" t="s">
+      <c r="J16" s="54"/>
+      <c r="K16" s="138"/>
+      <c r="L16" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="M16" s="89" t="s">
+      <c r="M16" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="9">
         <v>50</v>
       </c>
-      <c r="O16" s="69"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="21" t="s">
+      <c r="O16" s="55"/>
+      <c r="P16" s="138"/>
+      <c r="Q16" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="R16" s="80" t="s">
+      <c r="R16" s="66" t="s">
         <v>160</v>
       </c>
-      <c r="S16" s="81">
+      <c r="S16" s="67">
         <v>16</v>
       </c>
-      <c r="T16" s="88" t="s">
+      <c r="T16" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="U16" s="73"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="21" t="s">
+      <c r="U16" s="59"/>
+      <c r="V16" s="137"/>
+      <c r="W16" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="X16" s="80" t="s">
+      <c r="X16" s="66" t="s">
         <v>163</v>
       </c>
-      <c r="Y16" s="82">
+      <c r="Y16" s="68">
         <v>24</v>
       </c>
-      <c r="Z16" s="116" t="s">
+      <c r="Z16" s="102" t="s">
         <v>164</v>
       </c>
-      <c r="AA16" s="73"/>
+      <c r="AA16" s="59"/>
       <c r="AB16" s="162"/>
-      <c r="AC16" s="90"/>
-      <c r="AD16" s="91" t="s">
+      <c r="AC16" s="76"/>
+      <c r="AD16" s="77" t="s">
         <v>165</v>
       </c>
-      <c r="AE16" s="92">
+      <c r="AE16" s="78">
         <f>SUM(AE13:AE15)</f>
         <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="152"/>
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="81" t="s">
         <v>166</v>
       </c>
-      <c r="C17" s="89" t="s">
+      <c r="C17" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="79">
+      <c r="D17" s="65">
         <v>21</v>
       </c>
-      <c r="E17" s="64"/>
+      <c r="E17" s="50"/>
       <c r="F17" s="163"/>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="H17" s="117" t="s">
+      <c r="H17" s="103" t="s">
         <v>169</v>
       </c>
-      <c r="I17" s="118">
+      <c r="I17" s="104">
         <v>35</v>
       </c>
-      <c r="J17" s="68"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="90" t="s">
+      <c r="J17" s="54"/>
+      <c r="K17" s="138"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="76" t="s">
         <v>170</v>
       </c>
-      <c r="N17" s="91">
+      <c r="N17" s="77">
         <f>SUM(N14:N16)</f>
         <v>86</v>
       </c>
-      <c r="O17" s="69"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="21" t="s">
+      <c r="O17" s="55"/>
+      <c r="P17" s="138"/>
+      <c r="Q17" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="R17" s="80" t="s">
+      <c r="R17" s="66" t="s">
         <v>172</v>
       </c>
-      <c r="S17" s="81">
+      <c r="S17" s="67">
         <v>18</v>
       </c>
-      <c r="T17" s="88" t="s">
+      <c r="T17" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="U17" s="73"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="21" t="s">
+      <c r="U17" s="59"/>
+      <c r="V17" s="137"/>
+      <c r="W17" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="X17" s="80" t="s">
+      <c r="X17" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="Y17" s="119">
+      <c r="Y17" s="105">
         <v>24</v>
       </c>
-      <c r="Z17" s="116" t="s">
+      <c r="Z17" s="102" t="s">
         <v>162</v>
       </c>
-      <c r="AA17" s="73"/>
+      <c r="AA17" s="59"/>
       <c r="AB17" s="164" t="s">
         <v>26</v>
       </c>
-      <c r="AC17" s="65" t="s">
+      <c r="AC17" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="AD17" s="80" t="s">
+      <c r="AD17" s="66" t="s">
         <v>177</v>
       </c>
-      <c r="AE17" s="23">
+      <c r="AE17" s="9">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="152"/>
-      <c r="B18" s="95" t="s">
+      <c r="B18" s="81" t="s">
         <v>178</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D18" s="79">
+      <c r="D18" s="65">
         <v>14</v>
       </c>
-      <c r="E18" s="64"/>
+      <c r="E18" s="50"/>
       <c r="F18" s="163"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="104" t="s">
+      <c r="G18" s="89"/>
+      <c r="H18" s="90" t="s">
         <v>180</v>
       </c>
-      <c r="I18" s="105">
+      <c r="I18" s="91">
         <f>SUM(I15:I17)</f>
         <v>70</v>
       </c>
-      <c r="J18" s="68"/>
+      <c r="J18" s="54"/>
       <c r="K18" s="165" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="106" t="s">
+      <c r="L18" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="M18" s="19" t="s">
+      <c r="M18" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="N18" s="120">
+      <c r="N18" s="106">
         <v>21</v>
       </c>
-      <c r="O18" s="69"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="21" t="s">
+      <c r="O18" s="55"/>
+      <c r="P18" s="138"/>
+      <c r="Q18" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="R18" s="25" t="s">
+      <c r="R18" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="S18" s="81">
+      <c r="S18" s="67">
         <v>16</v>
       </c>
-      <c r="T18" s="121" t="s">
+      <c r="T18" s="107" t="s">
         <v>185</v>
       </c>
-      <c r="U18" s="73"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="94"/>
-      <c r="X18" s="90" t="s">
+      <c r="U18" s="59"/>
+      <c r="V18" s="137"/>
+      <c r="W18" s="80"/>
+      <c r="X18" s="76" t="s">
         <v>186</v>
       </c>
-      <c r="Y18" s="91">
+      <c r="Y18" s="77">
         <f>SUM(Y14:Y17)</f>
         <v>84</v>
       </c>
-      <c r="Z18" s="122"/>
-      <c r="AA18" s="123"/>
+      <c r="Z18" s="108"/>
+      <c r="AA18" s="109"/>
       <c r="AB18" s="164"/>
-      <c r="AC18" s="65" t="s">
+      <c r="AC18" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="AD18" s="80" t="s">
+      <c r="AD18" s="66" t="s">
         <v>188</v>
       </c>
-      <c r="AE18" s="23">
+      <c r="AE18" s="9">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="152"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="100" t="s">
+      <c r="B19" s="55"/>
+      <c r="C19" s="86" t="s">
         <v>189</v>
       </c>
-      <c r="D19" s="101">
+      <c r="D19" s="87">
         <f>SUM(D15:D18)</f>
         <v>70</v>
       </c>
-      <c r="E19" s="64"/>
-      <c r="F19" s="9" t="s">
+      <c r="E19" s="50"/>
+      <c r="F19" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="H19" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="I19" s="63">
+      <c r="I19" s="49">
         <v>14</v>
       </c>
-      <c r="J19" s="68"/>
+      <c r="J19" s="54"/>
       <c r="K19" s="165"/>
-      <c r="L19" s="21" t="s">
+      <c r="L19" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="M19" s="22" t="s">
+      <c r="M19" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="N19" s="23">
+      <c r="N19" s="9">
         <v>39</v>
       </c>
-      <c r="O19" s="124"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="21" t="s">
+      <c r="O19" s="110"/>
+      <c r="P19" s="138"/>
+      <c r="Q19" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="R19" s="80" t="s">
+      <c r="R19" s="66" t="s">
         <v>195</v>
       </c>
-      <c r="S19" s="81">
+      <c r="S19" s="67">
         <v>18</v>
       </c>
-      <c r="T19" s="95" t="s">
+      <c r="T19" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="U19" s="73"/>
-      <c r="V19" s="9" t="s">
+      <c r="U19" s="59"/>
+      <c r="V19" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="W19" s="21" t="s">
+      <c r="W19" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="X19" s="84" t="s">
+      <c r="X19" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="Y19" s="82">
+      <c r="Y19" s="68">
         <v>18</v>
       </c>
-      <c r="Z19" s="110"/>
-      <c r="AA19" s="73"/>
+      <c r="Z19" s="96"/>
+      <c r="AA19" s="59"/>
       <c r="AB19" s="164"/>
-      <c r="AC19" s="90"/>
-      <c r="AD19" s="91" t="s">
+      <c r="AC19" s="76"/>
+      <c r="AD19" s="77" t="s">
         <v>199</v>
       </c>
-      <c r="AE19" s="92">
+      <c r="AE19" s="78">
         <f>SUM(AE17:AE18)</f>
         <v>54</v>
       </c>
@@ -3951,362 +3888,362 @@
       <c r="A20" s="166" t="s">
         <v>200</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D20" s="63">
+      <c r="D20" s="49">
         <v>14</v>
       </c>
-      <c r="E20" s="64"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="45" t="s">
+      <c r="E20" s="50"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="I20" s="79">
+      <c r="I20" s="65">
         <v>39</v>
       </c>
-      <c r="J20" s="68"/>
+      <c r="J20" s="54"/>
       <c r="K20" s="165"/>
-      <c r="L20" s="94"/>
-      <c r="M20" s="90" t="s">
+      <c r="L20" s="80"/>
+      <c r="M20" s="76" t="s">
         <v>205</v>
       </c>
-      <c r="N20" s="91">
+      <c r="N20" s="77">
         <f>SUM(N18:N19)</f>
         <v>60</v>
       </c>
-      <c r="O20" s="124"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="94"/>
-      <c r="R20" s="90" t="s">
+      <c r="O20" s="110"/>
+      <c r="P20" s="138"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="76" t="s">
         <v>206</v>
       </c>
-      <c r="S20" s="91">
+      <c r="S20" s="77">
         <f>SUM(S15:S19)</f>
         <v>86</v>
       </c>
-      <c r="T20" s="125"/>
-      <c r="U20" s="73"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="21" t="s">
+      <c r="T20" s="111"/>
+      <c r="U20" s="59"/>
+      <c r="V20" s="138"/>
+      <c r="W20" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="X20" s="84" t="s">
+      <c r="X20" s="70" t="s">
         <v>208</v>
       </c>
-      <c r="Y20" s="82">
+      <c r="Y20" s="68">
         <v>18</v>
       </c>
-      <c r="Z20" s="116"/>
-      <c r="AA20" s="73"/>
+      <c r="Z20" s="102"/>
+      <c r="AA20" s="59"/>
     </row>
     <row r="21" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="166"/>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="D21" s="79">
+      <c r="D21" s="65">
         <v>39</v>
       </c>
-      <c r="E21" s="64"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="90" t="s">
+      <c r="E21" s="50"/>
+      <c r="F21" s="138"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="76" t="s">
         <v>211</v>
       </c>
-      <c r="I21" s="91">
+      <c r="I21" s="77">
         <f>SUM(I19:I20)</f>
         <v>53</v>
       </c>
-      <c r="J21" s="68"/>
-      <c r="K21" s="59"/>
-      <c r="O21" s="124"/>
-      <c r="P21" s="9" t="s">
+      <c r="J21" s="54"/>
+      <c r="K21" s="45"/>
+      <c r="O21" s="110"/>
+      <c r="P21" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="29" t="s">
+      <c r="Q21" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="R21" s="126" t="s">
+      <c r="R21" s="112" t="s">
         <v>213</v>
       </c>
-      <c r="S21" s="113">
+      <c r="S21" s="99">
         <v>50</v>
       </c>
-      <c r="T21" s="127" t="s">
+      <c r="T21" s="113" t="s">
         <v>214</v>
       </c>
-      <c r="U21" s="123"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="128" t="s">
+      <c r="U21" s="109"/>
+      <c r="V21" s="138"/>
+      <c r="W21" s="114" t="s">
         <v>215</v>
       </c>
-      <c r="X21" s="80" t="s">
+      <c r="X21" s="66" t="s">
         <v>216</v>
       </c>
-      <c r="Y21" s="82">
+      <c r="Y21" s="68">
         <v>45</v>
       </c>
-      <c r="Z21" s="114"/>
-      <c r="AB21" s="129"/>
+      <c r="Z21" s="100"/>
+      <c r="AB21" s="115"/>
     </row>
     <row r="22" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="166"/>
-      <c r="B22" s="94"/>
-      <c r="C22" s="90" t="s">
+      <c r="B22" s="80"/>
+      <c r="C22" s="76" t="s">
         <v>217</v>
       </c>
-      <c r="D22" s="91">
+      <c r="D22" s="77">
         <f>SUM(D20:D21)</f>
         <v>53</v>
       </c>
-      <c r="E22" s="64"/>
-      <c r="G22" s="130"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="131"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="129"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="132"/>
-      <c r="O22" s="124"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="94"/>
-      <c r="R22" s="90" t="s">
+      <c r="E22" s="50"/>
+      <c r="G22" s="116"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="117"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="115"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="118"/>
+      <c r="O22" s="110"/>
+      <c r="P22" s="138"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="76" t="s">
         <v>218</v>
       </c>
-      <c r="S22" s="91">
+      <c r="S22" s="77">
         <f ca="1">SUM(S21:S25)</f>
         <v>50</v>
       </c>
-      <c r="T22" s="133"/>
-      <c r="U22" s="123"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="90"/>
-      <c r="X22" s="91" t="s">
+      <c r="T22" s="119"/>
+      <c r="U22" s="109"/>
+      <c r="V22" s="138"/>
+      <c r="W22" s="76"/>
+      <c r="X22" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="Y22" s="91">
+      <c r="Y22" s="77">
         <f ca="1">SUM(Y19:Y25)</f>
         <v>81</v>
       </c>
-      <c r="Z22" s="134"/>
-      <c r="AA22" s="73"/>
-      <c r="AB22" s="129"/>
+      <c r="Z22" s="120"/>
+      <c r="AA22" s="59"/>
+      <c r="AB22" s="115"/>
     </row>
     <row r="23" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="135"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="129"/>
-      <c r="G23" s="130"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="131"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="132"/>
-      <c r="O23" s="124"/>
-      <c r="P23" s="136"/>
-      <c r="Q23" s="137"/>
-      <c r="R23" s="137"/>
-      <c r="S23" s="137"/>
-      <c r="T23" s="73"/>
-      <c r="U23" s="123"/>
-      <c r="V23" s="129"/>
-      <c r="W23" s="137"/>
-      <c r="X23" s="137"/>
-      <c r="Y23" s="137"/>
-      <c r="Z23" s="138"/>
-      <c r="AA23" s="138"/>
-      <c r="AB23" s="129"/>
+      <c r="A23" s="121"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="115"/>
+      <c r="G23" s="116"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="118"/>
+      <c r="O23" s="110"/>
+      <c r="P23" s="122"/>
+      <c r="Q23" s="123"/>
+      <c r="R23" s="123"/>
+      <c r="S23" s="123"/>
+      <c r="T23" s="59"/>
+      <c r="U23" s="109"/>
+      <c r="V23" s="115"/>
+      <c r="W23" s="123"/>
+      <c r="X23" s="123"/>
+      <c r="Y23" s="123"/>
+      <c r="Z23" s="124"/>
+      <c r="AA23" s="124"/>
+      <c r="AB23" s="115"/>
     </row>
     <row r="24" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="135"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="129"/>
-      <c r="G24" s="130"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="131"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="132"/>
-      <c r="O24" s="124"/>
-      <c r="P24" s="136"/>
-      <c r="R24" s="137"/>
-      <c r="S24" s="137"/>
-      <c r="T24" s="139"/>
-      <c r="U24" s="123"/>
-      <c r="V24" s="129"/>
-      <c r="W24" s="137"/>
-      <c r="X24" s="137"/>
-      <c r="Y24" s="137"/>
-      <c r="Z24" s="138"/>
-      <c r="AA24" s="138"/>
-      <c r="AB24" s="129"/>
+      <c r="A24" s="121"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="115"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="118"/>
+      <c r="O24" s="110"/>
+      <c r="P24" s="122"/>
+      <c r="R24" s="123"/>
+      <c r="S24" s="123"/>
+      <c r="T24" s="125"/>
+      <c r="U24" s="109"/>
+      <c r="V24" s="115"/>
+      <c r="W24" s="123"/>
+      <c r="X24" s="123"/>
+      <c r="Y24" s="123"/>
+      <c r="Z24" s="124"/>
+      <c r="AA24" s="124"/>
+      <c r="AB24" s="115"/>
     </row>
     <row r="25" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="140"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="129"/>
-      <c r="G25" s="130"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="131"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="132"/>
-      <c r="O25" s="124"/>
-      <c r="P25" s="136"/>
-      <c r="Q25" s="137"/>
-      <c r="R25" s="137"/>
-      <c r="S25" s="137"/>
-      <c r="T25" s="139"/>
-      <c r="U25" s="123"/>
-      <c r="V25" s="129"/>
-      <c r="W25" s="137"/>
-      <c r="X25" s="137"/>
-      <c r="Y25" s="137"/>
-      <c r="Z25" s="138"/>
-      <c r="AA25" s="138"/>
-      <c r="AB25" s="129"/>
+      <c r="A25" s="126"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="117"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="118"/>
+      <c r="O25" s="110"/>
+      <c r="P25" s="122"/>
+      <c r="Q25" s="123"/>
+      <c r="R25" s="123"/>
+      <c r="S25" s="123"/>
+      <c r="T25" s="125"/>
+      <c r="U25" s="109"/>
+      <c r="V25" s="115"/>
+      <c r="W25" s="123"/>
+      <c r="X25" s="123"/>
+      <c r="Y25" s="123"/>
+      <c r="Z25" s="124"/>
+      <c r="AA25" s="124"/>
+      <c r="AB25" s="115"/>
     </row>
     <row r="26" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="140"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="129"/>
-      <c r="J26" s="59"/>
-      <c r="O26" s="69"/>
-      <c r="P26" s="136"/>
-      <c r="U26" s="141"/>
-      <c r="AB26" s="129"/>
+      <c r="A26" s="126"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="115"/>
+      <c r="J26" s="45"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="122"/>
+      <c r="U26" s="127"/>
+      <c r="AB26" s="115"/>
     </row>
     <row r="27" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="140"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="129"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="132"/>
-      <c r="O27" s="69"/>
-      <c r="P27" s="136"/>
-      <c r="U27" s="141"/>
-      <c r="AB27" s="129"/>
+      <c r="A27" s="126"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="115"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="118"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="122"/>
+      <c r="U27" s="127"/>
+      <c r="AB27" s="115"/>
     </row>
     <row r="28" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="142"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="129"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="132"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="136"/>
-      <c r="U28" s="73"/>
-      <c r="AB28" s="129"/>
+      <c r="A28" s="128"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="115"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="118"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="122"/>
+      <c r="U28" s="59"/>
+      <c r="AB28" s="115"/>
     </row>
     <row r="29" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E29" s="64"/>
-      <c r="F29" s="129"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="132"/>
-      <c r="O29" s="69"/>
-      <c r="P29" s="136"/>
-      <c r="U29" s="73"/>
-      <c r="AB29" s="129"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="115"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="118"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="122"/>
+      <c r="U29" s="59"/>
+      <c r="AB29" s="115"/>
     </row>
     <row r="30" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="64"/>
-      <c r="F30" s="129"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="132"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="136"/>
-      <c r="U30" s="73"/>
-      <c r="AB30" s="143"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="115"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="118"/>
+      <c r="O30" s="55"/>
+      <c r="P30" s="122"/>
+      <c r="U30" s="59"/>
+      <c r="AB30" s="129"/>
     </row>
     <row r="31" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E31" s="64"/>
-      <c r="F31" s="129"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="132"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="136"/>
-      <c r="U31" s="73"/>
-      <c r="AB31" s="143"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="115"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="118"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="122"/>
+      <c r="U31" s="59"/>
+      <c r="AB31" s="129"/>
     </row>
     <row r="32" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E32" s="64"/>
-      <c r="F32" s="143"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="132"/>
-      <c r="O32" s="69"/>
-      <c r="P32" s="143"/>
-      <c r="U32" s="138"/>
-      <c r="AB32" s="143"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="129"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="118"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="129"/>
+      <c r="U32" s="124"/>
+      <c r="AB32" s="129"/>
     </row>
     <row r="33" spans="5:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E33" s="64"/>
-      <c r="F33" s="143"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="132"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="143"/>
-      <c r="U33" s="138"/>
-      <c r="AB33" s="62"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="129"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="118"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="129"/>
+      <c r="U33" s="124"/>
+      <c r="AB33" s="48"/>
     </row>
     <row r="34" spans="5:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E34" s="64"/>
-      <c r="F34" s="143"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="132"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="143"/>
-      <c r="U34" s="138"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="129"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="118"/>
+      <c r="O34" s="55"/>
+      <c r="P34" s="129"/>
+      <c r="U34" s="124"/>
     </row>
     <row r="35" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E35" s="64"/>
-      <c r="F35" s="142"/>
-      <c r="J35" s="68"/>
-      <c r="K35" s="61"/>
-      <c r="O35" s="124"/>
-      <c r="P35" s="62"/>
-      <c r="U35" s="138"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="128"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="47"/>
+      <c r="O35" s="110"/>
+      <c r="P35" s="48"/>
+      <c r="U35" s="124"/>
     </row>
     <row r="36" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E36" s="64"/>
-      <c r="J36" s="68"/>
-      <c r="O36" s="124"/>
-      <c r="U36" s="138"/>
+      <c r="E36" s="50"/>
+      <c r="J36" s="54"/>
+      <c r="O36" s="110"/>
+      <c r="U36" s="124"/>
     </row>
     <row r="37" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E37" s="102"/>
-      <c r="J37" s="59"/>
-      <c r="O37" s="124"/>
-      <c r="U37" s="144"/>
+      <c r="E37" s="88"/>
+      <c r="J37" s="45"/>
+      <c r="O37" s="110"/>
+      <c r="U37" s="130"/>
     </row>
     <row r="38" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E38" s="102"/>
-      <c r="J38" s="59"/>
-      <c r="O38" s="124"/>
-      <c r="U38" s="144"/>
+      <c r="E38" s="88"/>
+      <c r="J38" s="45"/>
+      <c r="O38" s="110"/>
+      <c r="U38" s="130"/>
     </row>
     <row r="39" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E39" s="102"/>
-      <c r="J39" s="59"/>
-      <c r="O39" s="62"/>
-      <c r="U39" s="144"/>
+      <c r="E39" s="88"/>
+      <c r="J39" s="45"/>
+      <c r="O39" s="48"/>
+      <c r="U39" s="130"/>
     </row>
     <row r="40" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E40" s="102"/>
-      <c r="J40" s="59"/>
-      <c r="U40" s="144"/>
+      <c r="E40" s="88"/>
+      <c r="J40" s="45"/>
+      <c r="U40" s="130"/>
     </row>
     <row r="41" spans="5:28" x14ac:dyDescent="0.25">
-      <c r="E41" s="60"/>
-      <c r="J41" s="61"/>
-      <c r="U41" s="145"/>
+      <c r="E41" s="46"/>
+      <c r="J41" s="47"/>
+      <c r="U41" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -4362,293 +4299,140 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ34"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="146" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="146" customWidth="1"/>
-    <col min="3" max="1024" width="14.42578125" style="146"/>
+    <col min="1" max="1" width="25.28515625" style="132" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="132" customWidth="1"/>
+    <col min="3" max="1024" width="14.42578125" style="132"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="133" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="148" t="s">
+      <c r="B1" s="134" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="135" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="150">
+      <c r="B2" s="136">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="149" t="s">
+      <c r="A3" s="135" t="s">
         <v>223</v>
       </c>
-      <c r="B3" s="150">
+      <c r="B3" s="136">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="149" t="s">
+      <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>224</v>
       </c>
-      <c r="B4" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="149" t="s">
+      <c r="B5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>225</v>
       </c>
-      <c r="B5" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="149" t="s">
+      <c r="B7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>226</v>
       </c>
-      <c r="B6" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="149" t="s">
+      <c r="B9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>227</v>
       </c>
-      <c r="B7" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="149" t="s">
+      <c r="B12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>228</v>
       </c>
-      <c r="B8" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="149" t="s">
+      <c r="B13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>229</v>
       </c>
-      <c r="B9" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="149" t="s">
-        <v>230</v>
-      </c>
-      <c r="B10" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="149" t="s">
-        <v>231</v>
-      </c>
-      <c r="B11" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="149" t="s">
-        <v>233</v>
-      </c>
-      <c r="B13" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="149" t="s">
+      <c r="B14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>234</v>
       </c>
-      <c r="B14" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="149" t="s">
-        <v>235</v>
-      </c>
-      <c r="B15" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="149" t="s">
-        <v>236</v>
-      </c>
-      <c r="B16" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="149" t="s">
-        <v>237</v>
-      </c>
-      <c r="B17" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="149" t="s">
-        <v>238</v>
-      </c>
-      <c r="B18" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="149" t="s">
-        <v>239</v>
-      </c>
-      <c r="B19" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="149" t="s">
-        <v>240</v>
-      </c>
-      <c r="B20" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="149" t="s">
-        <v>241</v>
-      </c>
-      <c r="B21" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="149" t="s">
-        <v>242</v>
-      </c>
-      <c r="B22" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="149" t="s">
-        <v>243</v>
-      </c>
-      <c r="B23" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="149" t="s">
-        <v>244</v>
-      </c>
-      <c r="B24" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="149" t="s">
-        <v>245</v>
-      </c>
-      <c r="B25" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="149" t="s">
-        <v>246</v>
-      </c>
-      <c r="B26" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="149" t="s">
-        <v>247</v>
-      </c>
-      <c r="B27" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="149" t="s">
-        <v>248</v>
-      </c>
-      <c r="B28" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="149" t="s">
-        <v>249</v>
-      </c>
-      <c r="B29" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="149" t="s">
-        <v>250</v>
-      </c>
-      <c r="B30" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="149" t="s">
-        <v>251</v>
-      </c>
-      <c r="B31" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="149" t="s">
-        <v>252</v>
-      </c>
-      <c r="B32" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="149" t="s">
-        <v>253</v>
-      </c>
-      <c r="B33" s="150">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="149" t="s">
-        <v>254</v>
-      </c>
-      <c r="B34" s="150">
-        <v>36</v>
+      <c r="B15">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>